<commit_message>
continuing work on text extraction
</commit_message>
<xml_diff>
--- a/output/process/no_geo.xlsx
+++ b/output/process/no_geo.xlsx
@@ -4603,16 +4603,16 @@
     <t>МШАГА, или МШАЖСКОЙ, погостъ Новогородскаго Намѣстничества и уѣзду. Въ ономъ бываетъ годовой съѣздъ для торговли въ пятницу предъ днемъ Св. Пророка Иліи.</t>
   </si>
   <si>
-    <t>МЫШКИНЪ, городъ Ярославскаго Намѣстничества. Въ немъ бываетъ годовая ярмарка въ Маіѣ мѣсяцѣ. Съѣзжаются купцы изъ ближнихъ городовъ, какъ-то изъ Ярославля, Ростова , Романова , Углича , Борисоглѣбска , Рыбинска, Мологи и слободы Норской.</t>
-  </si>
-  <si>
-    <t>МЯГКОЕ , село Тульскаго Намѣстничества въ Каширскомъ уѣздѣ. Въ ономъ во время десятой и одинадцатой пятницъ бываютъ ярмарки, на которыя товары въ продажу привозятъ изъ Каширы , Тулы , Серпухова , Венева и Зарайска по малому числу москотильной и мѣлочной; а отъ обывателей уѣздныхъ въ продажѣ бываетъ пенька , медъ, воскъ и деревянное издѣлье.</t>
-  </si>
-  <si>
-    <t>НАБДИНЪ, погостъ Псковскаго Намѣстничества въ Великолуцкомъ уѣздѣ. Здѣсь бываетъ годовая ярмарка Декабря 25 дня, на коей отъ обывателей продаются кожи, ленъ, пенька, медъ и прочія тому подобныя вещи; а отъ Великолуцкихъ, Торопецкихъ Псковскихъ купцовъ разные мѣлкіe шелковые товары.</t>
-  </si>
-  <si>
-    <t>НАРВА , городъ С. Петербургской Губерніи. Въ немъ еще по Шведскимъ учрежденіямъ положено въ годъ быть двумъ ярмаркамъ, въ Февралѣ и Iюлѣ</t>
+    <t>МЫШКИНЪ, городъ Ярославскаго Намѣстничества. Въ немъ бываетъ годовая ярмарка въ Маія мѣсяцѣ. Съѣзжаются купцы изъ ближнихъ городовъ, какъ - то изъ Ярославля, Ростова , Романова , Углича , Борисоглѣбка , Рыбинска, Мологи и слободы Норской.</t>
+  </si>
+  <si>
+    <t>МЯГКОЕ , село Тульскаго Намѣстничества въ Каширскомъ уѣздѣ. Въ ономъ во время десятой и одиннадцатой пятницъ бываютъ ярмарки, на которыя товары въ продажу привозятъ изъ Каширы , Тулы , Серпухова , Венева и Зарайска по малому числу москотильной и мѣлочной; а отъ обывателей уѣздныхъ въ продажѣ бываетъ пенька , медъ, воскъ и деревянное издѣлье.</t>
+  </si>
+  <si>
+    <t>НАБДИНЪ, погостъ Псковскаго Намѣстничества въ Великолуцкомъ уѣздѣ. Здѣсь бываетъ годовая ярмарка Декабря 25 дня, на коей отъ обывателей продаются кожи, ленъ, пенька, медъ и прочія тому подобныя вещи; а отъ Великолуцкихъ, Торопецкихъ Псковскихъ купцовъ разные мѣлкіе шелковые товары.</t>
+  </si>
+  <si>
+    <t>НАРВА , городъ С. Петербургской Губерніи Въ немъ еще по Шведскимъ учрежденіямъ положено въ годъ быть двумъ ярмаркамъ , въ февралѣ и Іюлѣ</t>
   </si>
   <si>
     <t>НАРОВЧАТЪ , городъ Пензенскаго Намѣстничества. Въ семъ городѣ бываетъ въ годъ три ярмарки : первая Іюня 29, вторая Іюля 20, третія Августа 6 дня, сверхъ Обыкновенныхъ каждонедѣльныхъ торговъ.</t>
@@ -7345,16 +7345,16 @@
     <t>МШАГА, или МШАЖСКОЙ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;погостъ&lt;/span&gt;&lt;span class="font0"&gt; Новогородскаго Намѣстничества и уѣзду. Въ ономъ бываетъ годовой съѣздъ для торговли въ пятницу предъ днемъ Св. Пророка Иліи.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>МЫШКИНЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Ярославскаго Намѣстничества. Въ немъ бываетъ годовая ярмарка въ Маіѣ мѣсяцѣ. Съѣзжаются купцы изъ ближнихъ городовъ, какъ-то изъ Ярославля, Ростова , Романова , Углича , Борисоглѣбска , Рыбинска, Мологи и слободы Норской.&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>МЯГКОЕ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Тульскаго Намѣстничества въ Каширскомъ уѣздѣ. Въ ономъ во время десятой и одинадцатой пятницъ бываютъ ярмарки, на которыя товары въ продажу привозятъ изъ Каширы , Тулы , Серпухова , Венева и Зарайска по малому числу москотильной и мѣлочной; а отъ обывателей уѣздныхъ въ продажѣ бываетъ пенька , медъ, воскъ и деревянное издѣлье.&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>НАБДИНЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;погостъ&lt;/span&gt;&lt;span class="font0"&gt; Псковскаго Намѣстничества въ Великолуцкомъ уѣздѣ. Здѣсь бываетъ годовая ярмарка Декабря 25 дня, на коей отъ обывателей продаются кожи, ленъ, пенька, медъ и прочія тому подобныя вещи; а отъ Великолуцкихъ, Торопецкихъ Псковскихъ купцовъ разные мѣлкіe шелковые товары.&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>НАРВА , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; С. Петербургской Губерніи. Въ немъ еще по Шведскимъ учрежденіямъ положено въ годъ быть двумъ ярмаркамъ, въ Февралѣ и Iюлѣ&lt;/span&gt;</t>
+    <t>МЫШКИНЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Ярославскаго Намѣстничества. Въ немъ бываетъ годовая ярмарка въ Маія мѣсяцѣ. Съѣзжаются купцы изъ ближнихъ городовъ, какъ - то изъ Ярославля, Ростова , Романова , Углича , Борисоглѣбка , Рыбинска, Мологи и слободы Норской.&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>МЯГКОЕ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Тульскаго Намѣстничества въ Каширскомъ уѣздѣ. Въ ономъ во время десятой и одиннадцатой пятницъ бываютъ ярмарки, на которыя товары въ продажу привозятъ изъ Каширы , Тулы , Серпухова , Венева и Зарайска по малому числу москотильной и мѣлочной; а отъ обывателей уѣздныхъ въ продажѣ бываетъ пенька , медъ, воскъ и деревянное издѣлье.&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>НАБДИНЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;погостъ&lt;/span&gt;&lt;span class="font0"&gt; Псковскаго Намѣстничества въ Великолуцкомъ уѣздѣ. Здѣсь бываетъ годовая ярмарка Декабря 25 дня, на коей отъ обывателей продаются кожи, ленъ, пенька, медъ и прочія тому подобныя вещи; а отъ Великолуцкихъ, Торопецкихъ Псковскихъ купцовъ разные мѣлкіе шелковые товары.&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>НАРВА , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; С. Петербургской Губерніи Въ немъ еще по Шведскимъ учрежденіямъ положено въ годъ быть двумъ ярмаркамъ , въ февралѣ и Іюлѣ&lt;/span&gt;</t>
   </si>
   <si>
     <t>НАРОВЧАТЪ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Пензенскаго Намѣстничества. Въ семъ городѣ бываетъ въ годъ три ярмарки : первая Іюня 29, вторая Іюля 20, третія Августа 6 дня, сверхъ Обыкновенныхъ каждонедѣльныхъ торговъ.&lt;/span&gt;</t>

</xml_diff>

<commit_message>
change in output from re-running scripts
</commit_message>
<xml_diff>
--- a/output/process/no_geo.xlsx
+++ b/output/process/no_geo.xlsx
@@ -3307,7 +3307,7 @@
     <t>АРХАНГЕЛЬСКЪ, главный городъ Намѣстничества сего имени. Въ немъ бываетъ каждой годъ ярмарка , которая начинается въ Маіѣ мѣсяцѣ съ приходомъ изъ Россіи барокъ, а изъ за моря кораблей; прямая же, или валовая начинается всегда въ Іюнѣ, а оканчивается въ первыхъ числахъ Октября ; на ней бываетъ торговля между иностранными и Россійскими купцами Россійскими и иностранными товарами , продолжающаяся во время мореплаванія, на которую ярмарку иностранные купцы всякіе иностранные товары чрезъ море на корабляхъ изъ чужихъ краевъ къ Архангельскому порту привозятъ; а Россійскіе въ тѣ мѣста отпускаютъ всякіе привозимые чрезъ верховые города водою и сухимъ путемъ Россійскіе, Китайскіе, Персидскіе, Турецкіе и прочіе Азіатскіе и другіе иностранные товары для народнаго употребленія, а не въ отвозъ въ чужіе край, а именно же: привозимыя вина Французскія, Португальскія, Гишпанскія и Нѣмецкія лучшія и ординарныя, ромъ, уксусъ, водка венгерская, еликсиръ , винной, камень , сукна Голландскія , Аглинскія , Гамбурскія, Шлезскія и прочія лучшія и ординарныя, лоскутья и покроми суконныя , стамеды , штофы и прочія тому подобныя шерстяныя матеріи ; штофы и прочія шелковыя и полушелковыя парчи и ленты , выбойки , полотна Голландскія, олово въ блюдахъ и торѣлкахъ и прочихъ мѣдочахъ , прутовое и въ слиткахъ , свинецъ, желѣзо листовое , иглы , ножи , вилки , ножницы и прочіе желѣзные товары; квасцы, ртуть, сѣра горючая , шелакъ, шпіатеръ, масло деревянное, винныя ягоды , изюмъ , коринка , смоквы, черносливъ, ядры мигдальныя , кофе , чай , перецъ , орѣшки чернильныя , сандалъ, сахаръ, лимоны, померанцы и прочіе фрукты свѣжіе и въ винѣ; гвоздика, корица и прочія пряныя зелья ; канфара, ладонъ росной и простой, изъ гумми разныхъ сортовъ; посуда стеклянная, цѣнинная и каменая , стеклы окончинныя и бутылки , сыры , патока черная, пшено сорочинское , свѣтильня бумажная, бобры, выдры, лисицы; краски , консель брусковая, киноварь, оринакъ; чулки шелковые и шерстяные , также и прочіе отпускные , какъ - то: хлѣбъ , сѣмя льняное, сало говяжье и ворванная смола, юфть, желѣзо полосное и гвозди желѣзные , пенька, ленѣ , рогожии кульки рогожные ; щетина , канаты и веревки пеньковыя и пакальныя , пряжа канатная, воскъ, гривы конскія , кости , кожи моржевыя , мыло ; мягкая рухлядь , куницы , горнаcтаи , россомахи , бѣлки , песцы, зайчины , мѣхи бѣльи и заячьи , кожи медвежьи, кошечьи и волчьи; полотна гладкія и салфеточныя широкія и узкія и брань уѣздной работы, Фламскія парусныя и равендукъ холстъ , хрящъ, посуда деревянная, свѣчи сальныя, языки говяжьи копченые, губа лиственная , клей Сибирской, кожи подошевныя и ворванныя, сукна сермяжныя и чирковыя туфли, чаи жуланъ и простой, бадьянъ, масло коровье льняное и конопляное, медъ сырецъ, рога оленьи , мясо говяжье соленое , семга соленая , пряники медовые.</t>
   </si>
   <si>
-    <t>АРХАНГЕЛЬСКОЕ, ЗМѢЕВКА тожь, село Рязанскаго Намѣстничества въ Донковскомъ уѣздѣ ; въ ономъ бываютъ въ году двѣ ярмарки: первая Февраля 2 въ день Срѣтенія Господня , внорая Ноября 8, въ день Архистратига Михаила. Сюда пріѣзжаютъ купцы съ разными мѣлочными. товарами.</t>
+    <t>АРХАНГЕЛЬСКОЕ, ЗМѢЕВКА тожь, село Рязанскаго Намѣстничества въ Донковскомъ уѣздѣ ; въ ономъ бываютъ въ году двѣ ярмарки: первая Февраля 2 въ день Срѣтенія Господня , вторая Ноября 8, въ день Архистратига Михаила. Сюда пріѣзжаютъ купцы съ разными мѣлочными. товарами.</t>
   </si>
   <si>
     <t>АСАКОВО , село Тульскаго Намѣстничества въ Веневскомъ уѣздѣ ; здѣсь бываетъ годовая ярмарка Іюля 8 числа; пріѣзжаютъ на оную разныхъ городовъ купцы съ товарами.</t>
@@ -3328,7 +3328,7 @@
     <t>БАЕВКА, село въ Сибири на вершинѣ рѣки Свіаги; въ ономъ всякое Воскресенье бываетъ торгъ.</t>
   </si>
   <si>
-    <t>БАЛАКЛЕЕВЪ , мѣстечко Харьковскаго Намѣстничества въ Изюмовскомъ уѣздѣ. Въ ономъ бываетъ въ году пять ярмарокъ: первая въ недѣлю Ваій, вторая Іюля 12, третія Августа 1, четвертая Сентября 23, пятая Декабря б чиселъ, на которыя пріѣзжаютъ купцы изъ разныхъ городовъ съ шелковыми , бумажными, гарусными и прочими товарами.</t>
+    <t>БАЛАКЛЕЕВЪ , мѣстечко Харьковскаго Намѣстничества въ Изюмовскомъ уѣздѣ. Въ ономъ бываетъ въ году пять ярмарокъ: первая въ недѣлю Ваій, вторая Іюля 12, третія Августа 1, четвертая Сентября 23, пятая Декабря 6 чиселъ, на которыя пріѣзжаютъ купцы изъ разныхъ городовъ съ шелковыми , бумажными, гарусными и прочими товарами.</t>
   </si>
   <si>
     <t>БАЛАХНА , городъ Нижегородскаго Намѣстничества. Въ ономъ бываютъ каждую недѣлю по середамъ и пятницамъ, а въ зимнее время и по воскресеньямъ торги, на которые крестьяне привозятъ болѣе хлѣбъ, съѣстные припасы и разныя для жителей потребности.</t>
@@ -3337,7 +3337,7 @@
     <t>БАРЫШЕВКА, мѣстечко Кіевскаго Намѣстничества въ Переяславскомъ уѣздѣ. Въ ономъ бываютъ въ году три ярмарки: первая Генваря 1, вторая Маія 9, третія Сентября 11 чиселъ, на которыхъ купцы торгуютъ разными мѣлочными товарами и привозимою изъ Донскихъ станицъ мѣлкою рыбою; а жители продаютъ рогатой скотъ, лошадей, хлѣбъ, смолу , горячее вино и Крымскую соль.</t>
   </si>
   <si>
-    <t>БАСАНЬ , мѣстечко того же Намѣстничества и уѣзду. Въ ономъ, кромѣ еженедѣльныхъ по понедѣльникамъ торговъ, бываетъ въ году пятярмарокъ: первая въ день Вознесенія Господня , вторая въ день Св. Апостоловъ Петра и Павла , третія въ день успенія Пресвятыя Богородицы, четвертая Сентября 2о, въ день Св. Евстафія, пятая Декабря 6, въ день Николая Чудотворца. Торгуютъ на оныхъ разными мѣлочными товарами и привозимою изъ Донскихъ станицъ мѣлкою рыбою. Жители продаютъ рогатой скотъ , лошадей , хлѣбъ, смолу, горячее вино и прочее; также привозятъ сюда для продажи жителямъ Крымскую соль.</t>
+    <t>БАСАНЬ , мѣстечко того же Намѣстничества и уѣзду. Въ ономъ, кромѣ еженедѣльныхъ по понедѣльникамъ торговъ, бываетъ въ году пятярмарокъ: первая въ день Вознесенія Господня , вторая въ день Св. Апостоловъ Петра и Павла , третія въ день успенія Пресвятыя Богородицы, четвертая Сентября 20, въ день Св. Евстафія, пятая Декабря 6, въ день Николая Чудотворца. Торгуютъ на оныхъ разными мѣлочными товарами и привозимою изъ Донскихъ станицъ мѣлкою рыбою. Жители продаютъ рогатой скотъ , лошадей , хлѣбъ, смолу, горячее вино и прочее; также привозятъ сюда для продажи жителямъ Крымскую соль.</t>
   </si>
   <si>
     <t>БАТРАКЪ, село Синбирскаго Намѣстничества ниже города Сызрани. Въ немъ съ 29 Іюня по 12 Іюля бываетъ годовая ярмарка, на которую особливо привозятъ много уральской рыбы и икры.</t>
@@ -3397,7 +3397,7 @@
     <t>БОГАЧКА, мѣстечко Кіевскаго Намѣстничества въ Миргородскомъ уѣздѣ. Въ ономъ бываетъ въ году двѣ ярмарки : одна въ день Сошествія Святаго Духа, а другая Сентября 1; торгуютъ на оныхъ пріѣзжіе изъ уѣзду жители разными мѣлочными товарами , тамъ родящимися и дѣлающимися, какъ-то хлѣбомъ, горячимъ виномъ,разнымъ скотомъ, дегтемъ, овчинами, кожами и проч. Иногда пріѣзжаютъ и Великороссійскіе купцы съ краснымъ товаромъ.</t>
   </si>
   <si>
-    <t>БОГОДУХОВЪ, городъ Харьковскаго Намѣстничества. Въ ономъ бываетъ въ году шесть ярмарокъ: первая на Сырной недѣлѣ , вторая въ постъ на похвальной недѣлѣ, третія на Вознесеніе , четвертая Іюля 20, пятая Августа 29, шестая Ноября Купцы пріѣзжаютъ на оныя изъ разныхъ Россійскихъ городовъ; привозятъ шелковые товары , парчи , позументы золотые и серебро въ дѣлѣ ; торгуютъ также скотомъ, лошадьми и прочимъ.</t>
+    <t>БОГОДУХОВЪ, городъ Харьковскаго Намѣстничества. Въ ономъ бываетъ въ году шесть ярмарокъ: первая на Сырной недѣлѣ , вторая въ постъ на похвальной недѣлѣ, третія на Вознесеніе , четвертая Іюля 20, пятая Августа 29, шестая Ноября 8. Купцы пріѣзжаютъ на оныя изъ разныхъ Россійскихъ городовъ; привозятъ шелковые товары , парчи , позументы золотые и серебро въ дѣлѣ ; торгуютъ также скотомъ, лошадьми и прочимъ.</t>
   </si>
   <si>
     <t>БОГОРОДИЦКЪ, городъ Тульскаго Намѣстничества. Въ семъ городѣ бываетъ ярмарка Іюля 7 и 8 дня, на которую изъ городовъ Тулы , Епифани, Кропивны , Дѣдилова, Ефремова и Донкова привозятъ мѣлочные красные товары , а оныхъ городовъ изъ уѣздовъ крестьяне колесы и лыки.</t>
@@ -3490,7 +3490,7 @@
     <t>БѢЛАЯ КОЛПЬ, село Московской Губерніи въ Волоколамскомъ уѣздѣ. Въ семъ селѣ бываетъ одна въ году ярмарка Августа 19 дня; торгуютъ одинъ день разными крестьянскими товарами.</t>
   </si>
   <si>
-    <t>БѢЛГОРОДЪ, городъ Курскаго Намѣстничества. Въ ономъ бываютъ три годовыя ярмарки: первая послѣ Святой недѣли въ десятую пятницу, вторая въ день Апостоловъ Петра и Павла, третія въ день Успвія Богородицы; да въ уѣздѣ онаго города бываютъ годовые торги въ Помѣщичьихъ слободахъ въ Петровской Мацвева, въ Троицкой Матюшкина, въ Сабыниной Брылкиной, въ Шебекиной Графа Генрикова, въ Алексѣевкѣ , Корчіюкъ тожь, економической , въ Зимовѣйкѣ и Бѣлей Князя Трубецкаго, въ Ефремовкѣ Герсевановой, въ Козмодемьянской Камышина, въ Михайловкѣ , Бекорюковка тожь , Бекорюкова, въ Вознесенской , Ивановка тожь , Бакшеева. Купцы на оные торги пріѣзжаютъ изъ близъ лежащихъ городовъ съ мѣлочными лавочными товарами.</t>
+    <t>БѢЛГОРОДЪ, городъ Курскаго Намѣстничества. Въ ономъ бываютъ три годовыя ярмарки: первая послѣ Святой недѣли въ десятую пятницу, вторая въ день Апостоловъ Петра и Павла, третія въ день Успенія Богородицы; да въ уѣздѣ онаго города бываютъ годовые торги въ Помѣщичьихъ слободахъ въ Петровской Мацвева, въ Троицкой Матюшкина, въ Сабыниной Брылкиной, въ Шебекиной Графа Генрикова, въ Алексѣевкѣ , Корчіюкъ тожь, економической , въ Зимовѣйкѣ и Бѣлей Князя Трубецкаго, въ Ефремовкѣ Герсевановой, въ Козмодемьянской Камышина, въ Михайловкѣ , Бекорюковка тожь , Бекорюкова, въ Вознесенской , Ивановка тожь , Бакшеева. Купцы на оные торги пріѣзжаютъ изъ близъ лежащихъ городовъ съ мѣлочными лавочными товарами.</t>
   </si>
   <si>
     <t>БѢЛИКИ , мѣстечко Екатеринославскаго Намѣстничества въ Полтавскомъ уѣздѣ. Въ ономъ бываетъ въ году три ярмарки.</t>
@@ -3628,7 +3628,7 @@
     <t>ВЫБОРЪ, пригородъ того же Намѣстничества. Здѣсь бываютъ годовыя ярмарки: первая въ день Сошествія Святаго Духа , вторая въ день Успенія Богородицы, третія въ день Воздвиженія. На оныя пріѣзжаютъ Торопецкіе купцы съ мѣлочнымъ товаромъ.</t>
   </si>
   <si>
-    <t>ВЫБОРГЪ, главный городъ Намѣстничества сего имени. Въ ономъ бываетъ въ каждое лѣто ярмарка, какъ въ городѣ приморскомъ; отсюда за море отпускаютъ доски, смолу , желѣзо , а получаютъ соль, табакъ , вина и прочее. Сверхъ сего бываетъ въ году еще двѣ ярмарки: первая Августа 24 вторая Сентября 21, на которыякрестьяне привозятъ по большей части рогатой скотъ, лошадей и съѣстные припасы.</t>
+    <t>ВЫБОРГЪ, главный городъ Намѣстничества сего имени. Въ ономъ бываетъ въ каждое лѣто ярмарка, какъ въ городѣ приморскомъ; отсюда за море отпускаютъ доски, смолу , желѣзо , а получаютъ соль, табакъ , вина и прочее. Сверхъ сего бываетъ въ году еще двѣ ярмарки: первая Августа 24, вторая Сентября 21, на которыякрестьяне привозятъ по большей части рогатой скотъ, лошадей и съѣстные припасы.</t>
   </si>
   <si>
     <t>ВЫСОКОЕ, село Московской Губерніи въ Волоколамскомъ уѣздѣ , въ которомъ есть небольшой рядъ , и въ ономъ производится продажа всякаго щепетильнаго товару, деревянной посуды , хлѣба и хмѣлю,</t>
@@ -3643,7 +3643,7 @@
     <t>ВЫЧУГА, село Костромскаго Намѣстничества въ уѣздѣ города Кинешмы. Здѣсь бываетъ годовая ярмарка въ Троицынъ день.</t>
   </si>
   <si>
-    <t>ВЫШГОРОДЪ , пригородъ Псковскаго Намѣстничества. Въ ономъ бываетъ въ году двѣ ярмарки : первая въ день, Бориса и Глѣба, а другая въ день Рождества Іоанна Предтечи.</t>
+    <t>ВЫШГОРОДЪ , пригородъ Псковскаго Намѣстничества. Въ ономъ бываетъ въ году двѣ ярмарки : первая въ день Бориса и Глѣба, а другая въ день Рождества Іоанна Предтечи.</t>
   </si>
   <si>
     <t>ВЫШГОРОДЪ, село Московской Губерніи въ Верейскомъ уѣздѣ. Въ ономъ бываютъ двѣ ярмарки въ году: первая въ десятую пятницу , вторая Іюля 2 числа ; на оныя пріѣзжаютъ купцы изъ городовъ Вереи, Можайска и Боровска , и множество сходится крестьянства ; торгуютъ всякими съѣстными припасами и крестьянскимъ товаромъ, какъ-то колесами, дегтемъ и тому подобнымъ.</t>
@@ -3694,7 +3694,7 @@
     <t>ГЖАТЬ, городъ Смоленскаго Намѣстничества. Въ семъ городѣ бываетъ годовая ярмарка , сверхъ каждонедѣльныхъ торговъ, Іюля 8 дня ; а въ селахъ бываетъ съѣздъ въ храмовые праздники , и въ каждомъ на одинъ только тотъ день.</t>
   </si>
   <si>
-    <t>ГЛЕМЯЗОВЪ, мѣстечко Кіевскаго Намѣстничества въ Переяславскомъ уѣздѣ. Въ ономъ бываетъ въ году четыре ярмарки : первая на Сырной недѣлѣ, вторая въ день Прополовенія, третія въ день Преображенія, четвертая въ день Введенія. Купцы пріѣзжаютъ на оныя изъ близъ лежащихъ городовъ съ красными крамными и прочими товарами, съ стеклянною и деревянною посудою, съ мѣлкою изъ Донскихъ станицѣ рыбою; жители продаютъ рогатой скотъ , лошадей, хлѣбѣ, смолу, горячее вино и прочее; привозятъ также сюда для продажи жителямъ Крымскую соль.</t>
+    <t>ГЛЕМЯЗОВЪ, мѣстечко Кіевскаго Намѣстничества въ Переяславскомъ уѣздѣ. Въ ономъ бываетъ въ году четыре ярмарки : первая на Сырной недѣлѣ, вторая въ день Преполовенія, третія въ день Преображенія, четвертая въ день Введенія. Купцы пріѣзжаютъ на оныя изъ близъ лежащихъ городовъ съ красными крамными и прочими товарами, съ стеклянною и деревянною посудою, съ мѣлкою изъ Донскихъ станицѣ рыбою; жители продаютъ рогатой скотъ , лошадей, хлѣбѣ, смолу, горячее вино и прочее; привозятъ также сюда для продажи жителямъ Крымскую соль.</t>
   </si>
   <si>
     <t>ГЛИНСКЪ , слобода Екатеринославскаго Намѣстничества. Въ оной бываетъ въ году три ярмарки.</t>
@@ -3814,13 +3814,13 @@
     <t>ДМИТРОВЪ, городъ Московской Губерніи. Въ ономъ бываетъ въ году одна ярмарка, которая начинается съ 15 Сентября , и продолжается недѣлю ; съ товарами пріѣзжаютъ изъ разныхъ ближиихъ городовъ , а именно изъ Москвы ,изъ Переславля Залѣснаго , изъ Ярославля; изъ Катина и изъ смѣжныхъ мѣстъ. Товары оные состоятъ въ щепетьѣ, шапкахъ, сапогахъ и прочей всякой мѣлочи; также торговыхъ дней въ недѣлѣ бываетъ два: понедѣльникъ и четвер токъ.</t>
   </si>
   <si>
-    <t>ДМИТРОВКА, ОЛЬШАНКА тожь , село Кіевскаго Намѣстничества около слободы Яб унева. Бываетъ здѣсь одна годовая ярмарка, на которую купцы пріѣзжаютъ съ разными товарами.</t>
+    <t>ДМИТРОВКА, ОЛЬШАНКА тожь , село Кіевскаго Намѣстничества около слободы Яблунева. Бываетъ здѣсь одна годовая ярмарка, на которую купцы пріѣзжаютъ съ разными товарами.</t>
   </si>
   <si>
     <t>ДМИТРОВСКАЯ, крѣпость Екатеринославскаго Намѣстничества. Въ оной бываетъ въ году три ярмарки.</t>
   </si>
   <si>
-    <t>ДОБРАЯ, слобода Воронежскаго Намѣстничества. Въ сей слободѣ въ году бываютъ три небольшія ярмарки: первая 9 Маія, вторая 26 Іюня, третія б Декабря, и продолжаются не болѣе какъ по одному, или по два Дни. Купцы на оныя привозятъ мѣлочные товары.</t>
+    <t>ДОБРАЯ, слобода Воронежскаго Намѣстничества. Въ сей слободѣ въ году бываютъ три небольшія ярмарки: первая 9 Маія, вторая 26 Іюня, третія 6 Декабря, и продолжаются не болѣе какъ по одному, или по два Дни. Купцы на оныя привозятъ мѣлочные товары.</t>
   </si>
   <si>
     <t>ДОМНИЦКОЙ, монастырь Черниговскаго Намѣстничества и уѣзду. При ономъ. бываетъ</t>
@@ -3946,7 +3946,7 @@
     <t>ЗЕМЛЯНСКЪ , городъ Воронежскаго Намѣстничества. Въ уѣздѣ сего города бываютъ ярмарки въ году въ трехъ селахъ; на оныя пріѣзжаютъ разныхъ городовъ Россійскіе купцы съ мѣлкимъ товаромъ.</t>
   </si>
   <si>
-    <t>ЗИНКОВЪ, или ЗѢНКОВЪ, городъ Черниговскаго Намѣстничества. Въ ономъ бываетъ въ годъ четыре ярмарки : первая Іюня 25 , въ день С. Іоанна Крестителя , вторая 15 Августа , въ день успенія Пресвятыя Богородицы, третія Октября 1, въ день Покрова Пресвятыя Богородицы , четвертая Декабря б, въ день Святителя Николая. На оныхъ торгуютъ разнымъ скотомъ, хлѣбомъ и съѣстными припасами. Здѣсь бываютъ и еженедѣльные торжки въ понедѣльникъ и пятокъ, и торгуютъ на оныхъ хлѣбомъ.</t>
+    <t>ЗИНКОВЪ, или ЗѢНКОВЪ, городъ Черниговскаго Намѣстничества. Въ ономъ бываетъ въ годъ четыре ярмарки : первая Іюня 25 , въ день С. Іоанна Крестителя , вторая 15 Августа , въ день успенія Пресвятыя Богородицы, третія Октября 1, въ день Покрова Пресвятыя Богородицы , четвертая Декабря 6, въ день Святителя Николая. На оныхъ торгуютъ разнымъ скотомъ, хлѣбомъ и съѣстными припасами. Здѣсь бываютъ и еженедѣльные торжки въ понедѣльникъ и пятокъ, и торгуютъ на оныхъ хлѣбомъ.</t>
   </si>
   <si>
     <t>ЗМѢЕВѢ, слобода Харьковскаго Намѣстничества въ уѣздѣ города Изюма. Въ оной бываютъ въ году три ярмарки : первая Іюня 29, въ день Св. Апостоловъ Петра и Павла, вторая Сентября 1, въ день Симеона Столпника, третія Октября 14, на день Параскевы. Купцы пріѣзжаютъ на оныя изъ разныхъ Россійскихъ городовъ съ шелковыми , шерстяными , бумажными и прочими товарами.</t>
@@ -3955,10 +3955,10 @@
     <t>ЗМѢТНЕВЪ, село Новогородскаго - Сѣверскаго Намѣстничества въ Сосницкомъ уѣздѣ. Обыватели онаго имѣютъ изрядной промыслъ бобрами , выдрами и рыбною въ Деснѣ ловлею.</t>
   </si>
   <si>
-    <t>ЗОЛОТОНОША , городъ Кіевскаго Намѣстничества. Въ немъ бываетъ въ году четыре ярмарки: первая въ Ѳомину недѣлю , вторая въ день Сошествія Свитаго Духа, третія въ день Рождества Богородицы , четвертая Декабря 6. Купцы пріѣзжаютъ на оныя изъ близъ лежащихъ городовъ съ красными крамными и прочими товарами , стеклянною и деревянною посудою и мѣлкою изъ Донскихъ станицъ рыбою; жители продаютъ рогатой скотъ, лошадей , хлѣбъ , смолу, горячее вино и прочее; привозятъ также сюда для лродажи жителямъ Крымскую соль.</t>
-  </si>
-  <si>
-    <t>ЗОЛОЧЕВЪ, городъ Харьковскаго Намѣстничества. Здѣсь бываютъ ярмарки Іюня 29, Августа 6, Декабря б ; торгуютъ купцы мѣлочнымъ товаромъ, виномъ, пивомъ, медомъ и прочимъ.</t>
+    <t>ЗОЛОТОНОША , городъ Кіевскаго Намѣстничества. Въ немъ бываетъ въ году четыре ярмарки: первая въ Ѳомину недѣлю , вторая въ день Сошествія Святаго Духа, третія въ день Рождества Богородицы , четвертая Декабря 6. Купцы пріѣзжаютъ на оныя изъ близъ лежащихъ городовъ съ красными крамными и прочими товарами , стеклянною и деревянною посудою и мѣлкою изъ Донскихъ станицъ рыбою; жители продаютъ рогатой скотъ, лошадей , хлѣбъ , смолу, горячее вино и прочее; привозятъ также сюда для лродажи жителямъ Крымскую соль.</t>
+  </si>
+  <si>
+    <t>ЗОЛОЧЕВЪ, городъ Харьковскаго Намѣстничества. Здѣсь бываютъ ярмарки Іюня 29, Августа 6, Декабря 6 ; торгуютъ купцы мѣлочнымъ товаромъ, виномъ, пивомъ, медомъ и прочимъ.</t>
   </si>
   <si>
     <t>ЗУБЦОВЪ, городъ Тверскаго Намѣстничества. Въ семъ городѣ бываютъ годовыя ярмарки : первая въ десятую пятницу по Пасхѣ , вторая Іюля 20, въ день Пророка Іліи, третія Августа 6, въ день Преображенія , четвертая Августа 15, въ день успенія , пятая 6 Декабря, шестая Маія 9, въ день Чудотворца Николая, седьмая Генваря 7, въ день Крестителя Іоанна, осьмая на Сырной недѣлѣ въ среду; торгуютъ окрестныхъ городовъ купцы - шелковыми , бумажными и прочими мѣлочными товарами, а большею частію съѣстными припасами.</t>
@@ -4003,7 +4003,7 @@
     <t>ИЗМАЙЛОВО , село Нижегородскаго Намѣстничества въ Арсамазскомъ уѣздѣ. Въ ономъ бываетъ одна въ г Ду ярмарка.</t>
   </si>
   <si>
-    <t>ИЗЮМЪ, городъ Харьковскаго Намѣстничества. Въ семъ городѣ бываетъ въ году четыре ярмарки: первая въ Маіѣ мѣсяцѣ въ день Преполовенія, вторая Іюня 24, въ день Рождества Іоанна Предтечи, третія Сентября 14, въ день Воздвиженія честнаго Креста, четвертая Октября 2б, въ день Великомученика Димитрія ; на оныя купцы пріѣзжаютъ изъ разныхъ городовъ съ шелковыми , бумажными , шерстяными и прочими товарами.</t>
+    <t>ИЗЮМЪ, городъ Харьковскаго Намѣстничества. Въ семъ городѣ бываетъ въ году четыре ярмарки: первая въ Маіѣ мѣсяцѣ въ день Преполовенія, вторая Іюня 24, въ день Рождества Іоанна Предтечи, третія Сентября 14, въ день Воздвиженія честнаго Креста, четвертая Октября 26, въ день Великомученика Димитрія ; на оныя купцы пріѣзжаютъ изъ разныхъ городовъ съ шелковыми , бумажными , шерстяными и прочими товарами.</t>
   </si>
   <si>
     <t>ИЛЬИНСКОЕ, село Тульскаго Намѣстничества въ Каширскомъ уѣздѣ. Здѣсь бываютъ торжки каждонедѣльно въ пятничные дни ; товары на оные привозятъ изъ уѣзда холсты льняные разные, да изъ городовъ Ярославля, Переславля Залѣснаго и Углича пріѣзжаютъ купцы съ мѣлочными всякими небогатыми товарами.</t>
@@ -4057,7 +4057,7 @@
     <t>КАМЕНЕЦЪ, мѣстечко Полотскаго Намѣстничества въ уѣздѣ города Динабурга. Въ семъ. мѣстѣ бываютъ три ярмарки въ году; торгуютъ Рижскаго Дворца крестьяне разными мѣлочными товарами, виномъ и пивомъ.</t>
   </si>
   <si>
-    <t>КАМЕНКА , слобода Харьковскаго Намѣстничества въ уѣздѣ города Изюма. Въ оной бываетъ въ году четыре ярмарки: первая ьъ день Алексія человѣка Божія , вторая въ день Великомученика Георгія, третія и четвертая во дни Николая Чудотворца лѣтняго и зимняго. На оныя купцы пріѣзжаютъ изъ разныхъ Россійскихъ городовъ съ шелковыми , бумажными , шерстяными товарами и прочимъ.</t>
+    <t>КАМЕНКА , слобода Харьковскаго Намѣстничества въ уѣздѣ города Изюма. Въ оной бываетъ въ году четыре ярмарки: первая въ день Алексія человѣка Божія , вторая въ день Великомученика Георгія, третія и четвертая во дни Николая Чудотворца лѣтняго и зимняго. На оныя купцы пріѣзжаютъ изъ разныхъ Россійскихъ городовъ съ шелковыми , бумажными , шерстяными товарами и прочимъ.</t>
   </si>
   <si>
     <t>КАМЫШНЯ, или КОМЫШНЯ , мѣстечко Кіевскаго Настничества въ Миргородскомъ уѣздѣ. Въ ономъ бываетъ въ году три ярмарки: первая въ недѣлю Ваій , вторая въ десятую послѣ Свѣтлаго Воскресенія пятницу , третія 26 Октября , въ день Св. Димитрія. На оныхъ торгуютъ рогатымъ скотомъ и лошадьми, а на еженедѣльныхъ въ понедѣльникъ и пятницу торгахъ торгуютъ пріѣзжіе изъ окольныхъ мѣстъ хлѣбомъ и съѣстными припасами.</t>
@@ -4462,7 +4462,7 @@
     <t>МАЛОЙ АРХАНГЕЛЬСКЪ, городъ Орловскаго Намѣстничества. Въ немъ бываетъ дважды въ недѣлю съѣздъ.</t>
   </si>
   <si>
-    <t>МАЛОЙ ЯРОСЛАВЕЦЪ, городъ Калужскаго Намѣстничества. Въ немъ бываютъ въ годъ ярмарки Апрѣля 23, Маія 9, Ноября 26, Декабря б и въ десятую пятницу по Пасхѣ , на которыя пріѣзжаютъ купцы изъ Боровска, Вереи и Серпухова съ шелковыми и бумажными платками , китайками , выбойками, чаемъ, сахаромъ, кофіемъ и разными москотильными товарами ; а главную часть сего торгу составляютъ окрестные жители, которые привозятъ съѣстные припасы и деревенскія издѣлья.</t>
+    <t>МАЛОЙ ЯРОСЛАВЕЦЪ, городъ Калужскаго Намѣстничества. Въ немъ бываютъ въ годъ ярмарки Апрѣля 23, Маія 9, Ноября 26, Декабря 6 и въ десятую пятницу по Пасхѣ , на которыя пріѣзжаютъ купцы изъ Боровска, Вереи и Серпухова съ шелковыми и бумажными платками , китайками , выбойками, чаемъ, сахаромъ, кофіемъ и разными москотильными товарами ; а главную часть сего торгу составляютъ окрестные жители, которые привозятъ съѣстные припасы и деревенскія издѣлья.</t>
   </si>
   <si>
     <t>МАЛЫКОВА, мѣстечко Полотскаго Намѣстничества въ уѣздѣ города Динабурга. Въ семъ мѣстѣ бываетъ въ году одна ярмарка; торгуютъ Рижскаго Дворца крестьяне разными мѣлочными товарами, виномъ и пивомъ.</t>
@@ -4510,7 +4510,7 @@
     <t>МЕРЕХВА, мѣстечко Харьковскаго Намѣстничества и уѣзду. Здѣсь бываютъ ярмарки Іюня 24, Августа 6; торгуютъ купцы мѣлочными, товарами , виномъ, пивомъ, медомъ и прочимъ.</t>
   </si>
   <si>
-    <t>МЕХОНСКОЙ , острогъ Уфимскаго Намѣстничества въ Челябинскомъ уѣздѣ. Здѣсь бываетъ ярмарка Декабря 25 и Іюля 2о; торгуютъ мѣлочнымъ товаромъ.</t>
+    <t>МЕХОНСКОЙ , острогъ Уфимскаго Намѣстничества въ Челябинскомъ уѣздѣ. Здѣсь бываетъ ярмарка Декабря 25 и Іюля 20; торгуютъ мѣлочнымъ товаромъ.</t>
   </si>
   <si>
     <t>МЕЩОВСКЪ, городъ Калужскаго Намѣстничества, Здѣсь бываетъ одна въ году ярмарка Іюля 29 дня; торгъ продолжается три дни ; на оную пріѣзжаютъ изъ разныхъ городовъ купцы со всякими товарами, а по большей части крестьяне съ Пенькою и хлѣбомъ.</t>
@@ -4630,7 +4630,7 @@
     <t>НАСПИЩИ, село Тульскаго Намѣстничества въ уѣздѣ города Алексина. Здѣсь бываетъ ярмарка Маія 2 и Іюля 24 дня; торгуютъ купцы до крестьянъ надлежащими товарами.</t>
   </si>
   <si>
-    <t>НЕВЕЛЬ , городъ Полотскаго Намѣстничества. Въ немъ бываютъ въ году четыре ярмарки: первая въ день Богоявленія, вторая въ первую недѣлю великаго поста, третія въ пятокъ Пктъ днемъ Пророка Иліи, четвертая Декабря 6 дня.</t>
+    <t>НЕВЕЛЬ , городъ Полотскаго Намѣстничества. Въ немъ бываютъ въ году четыре ярмарки: первая въ день Богоявленія, вторая въ первую недѣлю великаго поста, третія въ пятокъ предъ днемъ Пророка Иліи, четвертая Декабря 6 дня.</t>
   </si>
   <si>
     <t>НЕЛЬЯНСКОЙ , желѣзной заводъ Пермскаго Намѣстничества въ Екатеринбургскомъ уѣздѣ. Здѣсь бываетъ въ день Святыхъ Апостоловъ Петра и Павла нарочитая ярмарка прoдолжающаяся нѣсколько дней на которую съѣзжается много купцовъ изъ близъ лежащихъ городовъ , а именно: Екатеринбурга , Верхотурья, Туринска, Тюмени , которые , какъ и тамошніе жители , разными Россійскими , Сибирскими и Китайскими товарами торгуютъ.</t>
@@ -4723,7 +4723,7 @@
     <t>ОПОЧКА, городъ Псковскаго Намѣстничества. Въ семъ городѣ бываетъ въ году три ярмарки.</t>
   </si>
   <si>
-    <t>ОПОШНОЕ, мѣстечко Черниговскаго Намѣстничества въ Гадяцкомъ уѣздѣ. Въ ономъ бываетъ въ году четыре ярмарки : первая въ недѣлю Ѳомину, вторая въ десятую пятницу, третія Августа б, въ день Преображенія Господня, четвертая Октября 29, въ день Св. Димитрія ; на оныхъ торгуютъ разнымъ скотомъ, хлѣбомъ и съѣстными припасами. Здѣсь бываютъ еженедѣльные торжки въ понедѣльникъ и пятокъ, и торгуютъ большею частію хлѣбомъ.</t>
+    <t>ОПОШНОЕ, мѣстечко Черниговскаго Намѣстничества въ Гадяцкомъ уѣздѣ. Въ ономъ бываетъ въ году четыре ярмарки : первая въ недѣлю Ѳомину, вторая въ десятую пятницу, третія Августа 6, въ день Преображенія Господня, четвертая Октября 29, въ день Св. Димитрія ; на оныхъ торгуютъ разнымъ скотомъ, хлѣбомъ и съѣстными припасами. Здѣсь бываютъ еженедѣльные торжки въ понедѣльникъ и пятокъ, и торгуютъ большею частію хлѣбомъ.</t>
   </si>
   <si>
     <t>ОПУШКА, отчина разныхъ Господъ Тамбовскаго Намѣстничества въ Шатскомъ уѣздѣ. Здѣсь бываетъ въ году ярмарка 8 Іюля; торгуютъ разными товарами , какъ - то пенькою , разнымъ холстомъ медомъ, саломъ и прочимъ.</t>
@@ -4792,7 +4792,7 @@
     <t>ПЕРЕВОЛОЧНА, мѣстечко Екатеринославскаго Намѣстничества. Въ ономъ бываетъ въ году двѣ ярмарки.</t>
   </si>
   <si>
-    <t>ПЕРЕКОПЕЦЪ , мѣстечко въ уѣздѣ города Харькова. Здѣсь бываетъ ярмарка Марта 9, Маія б и Ноября 8, торгуютъ купцы мѣлочными товарами, виномъ , пивомъ , медомъ и прочимъ.</t>
+    <t>ПЕРЕКОПЕЦЪ , мѣстечко въ уѣздѣ города Харькова. Здѣсь бываетъ ярмарка Марта 9, Маія 6 и Ноября 8, торгуютъ купцы мѣлочными товарами, виномъ , пивомъ , медомъ и прочимъ.</t>
   </si>
   <si>
     <t>ПЕРЕМЫШЛЬ , городъ Калужскаго Намѣстничества. Здѣсь бываетъ годовая ярмарка сверхъ обыкновенныхъ торговъ въ десятую пятницу по Пасхѣ; привозятъ на продажу хдѣбъ, пеньку , хмѣль и прочее.</t>
@@ -4828,7 +4828,7 @@
     <t>ПЕТРОВСКОЕ, село Орловскаго Намѣстничества въ Елецкомъ уѣздѣ. Здѣсь бываетъ ярмарка Іюня 19 числа; на оной торгуютъ Елецкіе купцы и другихъ городовъ съ уѣздными обывателями всякими разными мѣлочными товарами; а обыватели продаютъ купцамъ и своей братьи лошадей, скотину, холстъ и съѣстные всякіе припасы и рукодѣлье.</t>
   </si>
   <si>
-    <t>ПЕТРОМА, село Ярославскаго Намѣстничества въ Пошехонскомъ уѣздѣ. Въ ономъ бываютъ двѣ годовыя ярмарки: первая Троецкая, вторая Ивановская , то есть 26 Сентября; пріѣзжаютъ на оныя купцы изъ сосѣдственныхъ городовъ съ разными шелковыми мѣлочными и прочими товарами.</t>
+    <t>ПЕТРОМА, село Ярославскаго Намѣстничества въ Пошехонскомъ уѣздѣ. Въ ономъ бываютъ двѣ годовыя ярмарки: первая Троицкая, вторая Ивановская , то есть 26 Сентября; пріѣзжаютъ на оныя купцы изъ сосѣдственныхъ городовъ съ разными шелковыми мѣлочными и прочими товарами.</t>
   </si>
   <si>
     <t>ПЕТРОПАВЛОВСКОЙ , шанцъ Екатеринославскаго Намѣстничества. Въ ономъ бываетъ въ годъ четыре ярмарки.</t>
@@ -4888,7 +4888,7 @@
     <t>ПОЛТАВА , городъ Екатеринославскаго Намѣстничества. Въ ономъ бываетъ въ году четыре ярмарки : первая въ сплошную недѣлю , вторая Маія 9, Николаевская , третія Іюля 20, Ильинская, четвертая Сентября 14, Воздвиженская. На оныя пріѣзжаютъ Великороссійскіе , Малороссійскіе и иностранные , изъ Польши , Шлезіи, Гданска, Царя - Града и изъ всей Турецкой области купцы и промышленники со всякими знатными и мѣлочными товарами. Купечество сего города отправляетъ во всѣ оныя мѣста родящіеся у нихъ и въ уѣздѣ продукты, какъ - то скотъ , масло , лошадей и другіе , холстъ, канаты и пушные разнаго рода товары. На еженедѣльные торги собираются въ оной городъ уѣздные жители, и торгуютъ Россійскими продуктами.</t>
   </si>
   <si>
-    <t>ПОНОРНИЦА , мѣстечко Черниговскаго Намѣстничества и уѣзду. Въ ономъ бываетъ въ году Двѣ ярмарки : первая Апрѣля 23, вторая Сентября чиселъ; торгуютъ на оныхъ и еженедѣльныхъ торгахъ пріѣзжіе изъ ближнихъ городовъ купцы мѣлочными товарами , а окольные жители тутошними произрастаніями и рукодѣліемъ, какъ - то деревянною посудою, неводными нитками , также скотомъ и прочими съѣстными припасами.</t>
+    <t>ПОНОРНИЦА , мѣстечко Черниговскаго Намѣстничества и уѣзду. Въ ономъ бываетъ въ году Двѣ ярмарки : первая Апрѣля 23, вторая Сентября 8 чиселъ; торгуютъ на оныхъ и еженедѣльныхъ торгахъ пріѣзжіе изъ ближнихъ городовъ купцы мѣлочными товарами , а окольные жители тутошними произрастаніями и рукодѣліемъ, какъ - то деревянною посудою, неводными нитками , также скотомъ и прочими съѣстными припасами.</t>
   </si>
   <si>
     <t>ПОРѢЧЬЕ , городъ Смоленскаго Намѣстничества. Въ ономъ бываетъ въ году двѣ ярмарки : первая Іюня мѣсяца въ десятую пятницу, вторая Сентября 8, въ день Рождества Богородицы ; купцы пріѣзжаютъ изъ близъ лежащихъ городовъ съ разными товарами.</t>
@@ -4900,7 +4900,7 @@
     <t>ПОТОКЪ, мѣстечко Кіевскаго Намѣстничества въ Миргородскомъ уѣздѣ. Въ ономъбываютъ въ годъ двѣ ярмарки: дпа Іюня 24, а другая Октября 6 чиселъ. Торгуютъ на оныхъ пріѣзжіе изъ уѣзду жители разными мѣлочными товарами , дамъ родящимися и дѣлающимися, какъ - то хлѣбомъ, горячимъ виномъ, разнымъ скотомъ, овчинами, кожами и проч. Иногда пріѣзжаютъ и Великороссійскіе купцы съ краснымъ товаромъ.</t>
   </si>
   <si>
-    <t>ПОЧИНКИ, село Пензенскаго Намѣстничества въ Саранскомъ уѣздѣ. Бываетъ здѣсь ярмарка въ послѣднихъ числахъ юля; привозятъ купцы разные мѣлочные шелковые товары.</t>
+    <t>ПОЧИНКИ, село Пензенскаго Намѣстничества въ Саранскомъ уѣздѣ. Бываетъ здѣсь ярмарка въ послѣднихъ числахъ Іюля; привозятъ купцы разные мѣлочные шелковые товары.</t>
   </si>
   <si>
     <t>ПОЧИНКИ , городъ Нижегородскаго Намѣстничества. Въ емъ, кромѣ еженедѣльнаго по четвергамъ торгу, бываетъ въ одъ Маія 25 дня ярмарка, на вторую пріѣзжаютъ изъ ближнихъ городовъ купцы съ мѣлочными шелковыми товарами, крестьяне привозить бывшею  хлѣбъ, лѣсъ и деревянную посуду.</t>
@@ -4954,7 +4954,7 @@
     <t>РАМЕНЬЕ, село Московской Губерніи въ Волоколамскомъ уѣздѣ. Здѣсь бываютъ въ году ярмарки Іюня 24 и 18 Сентября ; торгуютъ по одному дню разными крестьянскими товарами.</t>
   </si>
   <si>
-    <t>РАТКОВКА, слобода Харьковскаго Намѣстничества въ уѣздѣ города Изюма. Въ оной бываютъ въ году три ярмарки: Первая на Вознесеніе Господне , вторая Августа б , на Преображеніе , третія Октября 1, въ день Покрова. Купцы на оныя пріѣзжаютъ изъ разныхъ городовъ съ шелковыми , бумажными , гарусными и прочими товарами.</t>
+    <t>РАТКОВКА, слобода Харьковскаго Намѣстничества въ уѣздѣ города Изюма. Въ оной бываютъ въ году три ярмарки: Первая на Вознесеніе Господне , вторая Августа 6 , на Преображеніе , третія Октября 1, въ день Покрова. Купцы на оныя пріѣзжаютъ изъ разныхъ городовъ съ шелковыми , бумажными , гарусными и прочими товарами.</t>
   </si>
   <si>
     <t>РАТСБУРГЪ, отчина Меньшикова въ Екатеринославскомъ Намѣстничествѣ. Здѣсь бываютъ двѣ ярмарки , а именно : первая Троицкая, которая прежде была въ Лебединскомъ Троицкомъ монастырѣ , и переведена въ тое отчину; а другая въ той же отчинѣ Покровская , Октября і дня ; да сверхъ того бываютъ понедѣльные и временные торжки , на кои пріѣзжаютъ изъ ближнихъ городовъ купцы и изъ уѣздовъ крестьяне съ хлѣбомъ и прочею мѣлочью.</t>
@@ -5272,7 +5272,7 @@
     <t>ТЕПЛОГОРСКАЯ БОГОРОДИЦКАЯ , пустыня Вологодскаго Намѣстничества въ уѣздѣ Устюга Великаго. Здѣсь бываетъ въ году одна ярмарка, на которую пріѣзжаютъ купцы изъ разныхъ городовъ по большей части съ мѣлочными товарами.</t>
   </si>
   <si>
-    <t>ТЕРЕШКОВО, село Тверскаго Намѣстничества въ Зубцовскомъ уѣздѣ. Въ немъ бываетъ годовая ярмарка Маія 2о, въ день Алексѣя Митрополита; на оную пріѣзжаютъ купцы изъ окрестныхъ ближнихъ городовъ съ мѣлочными шелковыми и прочими товарами.</t>
+    <t>ТЕРЕШКОВО, село Тверскаго Намѣстничества въ Зубцовскомъ уѣздѣ. Въ немъ бываетъ годовая ярмарка Маія 20, въ день Алексѣя Митрополита; на оную пріѣзжаютъ купцы изъ окрестныхъ ближнихъ городовъ съ мѣлочными шелковыми и прочими товарами.</t>
   </si>
   <si>
     <t>ТЕРЯЕВО, село Московской Губерніи въ Рузскомъ уѣздѣ. Въ немъ бываетъ годовая ярмарка въ день Святаго Пророка Иліи.</t>
@@ -5305,7 +5305,7 @@
     <t>ТОМАРОВКА, слобода въ уѣздѣ города Карпова. Въ оной бываетъ ярмарка послѣ Рождества на всеѣдной недѣлѣ въ пятницу, Маія 9, Іюля 8, Декабря 6, и продолжаются оныя по одному дню. Купцы пріѣзжаютъ изъ окрестныхъ городовъ съ мѣлочными товарами.</t>
   </si>
   <si>
-    <t xml:space="preserve">ТОРЖОКЪ, съ 1775 году городъ Тверскаго Намѣстничества. Здѣсь бываютъ въ году три ярмарки : первая Генваря 6, вторая первой недѣли великагоста въ Воскресенье, третія Сентября 15 числа.   </t>
+    <t xml:space="preserve">ТОРЖОКЪ, съ 1775 году городъ Тверскаго Намѣстничества. Здѣсь бываютъ въ году три ярмарки : первая Генваря 6, вторая первой недѣли великагопоста въ Воскресенье, третія Сентября 15 числа.   </t>
   </si>
   <si>
     <t>ТОРОПЕЦЪ, съ 1777 году городъ Псковскаго Намѣстничества. Въ немъ случается въ году одна указная ярмарка въ Iюлѣ мѣсяцѣ въ пятокъ, предъ праздникомъ Пророка Иліи, на которую по большей части съѣзжаются крестьяне изъ ближнихъ деревень съ мѣлочнымъ крестьянскимъ товаромъ и рукодельемъ.</t>
@@ -5338,7 +5338,7 @@
     <t>ТУЛА, съ 1777 году главный городъ Намѣстничества сего имени. Здѣсь ярмарка бываетъ въ году два раза: I) при церкви Покрова Пресвятыя Богородицы , въ десятую отъ Святой недѣли пятницу; вторая Іюня 8 дня, при состоящемъ за городовымъ замкомъ Казанскомъ Соборѣ. Для складки привозимыхъ товаровъ имѣются подъ Тульскимъ Магистратомъ въ нижнемъ департаментѣ, также и особь построенныя палатки. Съ товарами на ярмарки постороннаго съѣзда не бываетъ, а отправляются только тамошними. Въ недѣлѣ два торга, въ понедѣльникъ и четвертокъ.</t>
   </si>
   <si>
-    <t>ТУРЕЦКАЯ треть, или волость Вологодскаго Намѣстничества въ уѣздѣ города Яренска. Здѣсь бываетъ ярмарка Февраля съ 15 дня по Мартъ мѣсяцъ; скупаютъ здѣсь купцы по большей части заготовленную и свезенную сюда крестьянами рыбу.</t>
+    <t>ТУРЕЦКАЯ треть, или волость Вологодскаго Намѣстничества въ уѣздѣ города Яренска. Здѣсь бываетъ ярмарка Февраля съ 15 дня по Мартѣ мѣсяцъ; скупаютъ здѣсь купцы по большей части заготовленную и свезенную сюда крестьянами рыбу.</t>
   </si>
   <si>
     <t>ТУРИНСКЪ, съ 1782 году городъ Тобольскаго Намѣстничества. Здѣсь бываютъ знатные торговые съѣзды по вся воскресные дни.</t>
@@ -5461,7 +5461,7 @@
     <t>ХРУЩОВО, село Рязанскаго Намѣстничества въ уѣздѣ города Донкова. Здѣсь бываютъ въ году двѣ ярмарки: первая Маія 9, вторая Августа 16 дня; пріѣзжаютъ на оныя купцы съ разными мѣлочными товарами , также и крестьянство.</t>
   </si>
   <si>
-    <t>ЦАРЕВЪ БОРИСОВЪ, городокъ Харьковскаго Намѣстничества въ уѣздѣ города Изюма. Въ ономъ бываетъ въ году четыре ярмарки : первая на всеѣдной недѣлѣ, вторая въ недѣлю Мѵроносицъ , третія послѣ Святой недѣли въ девятую пятницу, четвертая Ноября 8, въ день Архистратига Михаила; купцы пріѣзжаютъ на оныя изъ разныхъ Россійскихъ городовъ съ шелковыми , бумажными , гарусными и прочими товарами.</t>
+    <t>ЦАРЕВЪ БОРИСОВЪ, городокъ Харьковскаго Намѣстничества въ уѣздѣ города Изюма. Въ ономъ бываетъ въ году четыре ярмарки : первая на всеѣдной недѣлѣ, вторая въ недѣлю Мироносицъ , третія послѣ Святой недѣли въ девятую пятницу, четвертая Ноября 8, въ день Архистратига Михаила; купцы пріѣзжаютъ на оныя изъ разныхъ Россійскихъ городовъ съ шелковыми , бумажными , гарусными и прочими товарами.</t>
   </si>
   <si>
     <t>ЦАРИЧЕНКА , мѣстечко Екатеринославскаго Намѣстничества въ Полтавскомъ уѣздѣ. Въ ономъ бываютъ въ году три ярмарки.</t>
@@ -5488,7 +5488,7 @@
     <t>ЧАУСЫ, съ 1778 году городъ Могилевскаго Намѣстничества Здѣсь бываетъ одна годовая ярмарка.</t>
   </si>
   <si>
-    <t>ЧЕЛЯБИНСКЪ, съ 1782 году городъ Уфимскаго Намѣстничества , лежащій на рѣкѣ Міясѣ, отъ Далматовскаго монастыря во стѣ пятидесяти четырехъ верстахъ, въ самой срединѣ Башкирцевъ, можетъ со временемъ вразсужденіи торговъ сдѣлаться знатнымъ мѣстомъ; ибо намѣреніе принято было нетокмо для большей способности ради Башкирцевъ тамъ завести ярмарку, но еще и купечество изъ Великой Бухаріи, какъ въ Оренбургъ, такъ отчасти и туда перевести. Здѣсь бываютъ въ году двѣ ярмарки: первая Маія 9, вторая Декабря б дня.</t>
+    <t>ЧЕЛЯБИНСКЪ, съ 1782 году городъ Уфимскаго Намѣстничества , лежащій на рѣкѣ Міясѣ, отъ Далматовскаго монастыря во стѣ пятидесяти четырехъ верстахъ, въ самой срединѣ Башкирцевъ, можетъ со временемъ вразсужденіи торговъ сдѣлаться знатнымъ мѣстомъ; ибо намѣреніе принято было нетокмо для большей способности ради Башкирцевъ тамъ завести ярмарку, но еще и купечество изъ Великой Бухаріи, какъ въ Оренбургъ, такъ отчасти и туда перевести. Здѣсь бываютъ въ году двѣ ярмарки: первая Маія 9, вторая Декабря 6 дня.</t>
   </si>
   <si>
     <t>ЧЕНБАРЪ, съ 1780 году городъ Пензенскаго Намѣстничества. Въ ономъ бываетъ въ году ярмарка въ десятую пятницу по Пасхѣ; купцы пріѣзжаютъ изъ близъ лежащихъ городовъ съ недорогими товарами.</t>
@@ -5512,7 +5512,7 @@
     <t>ЧЕРНАВСКЪ, слобода Воронежскаго Намѣстничества. Здѣсь бываетъ одна въ году ярмарка въ день Срѣтенія Иконы Владимірскія Богородицы , то есть Іюня 23 дня; на оную пріѣзжаютъ купцы изъ ближнихъ городовъ съ мѣлкими товарами, и продолжается оная только половину дня.</t>
   </si>
   <si>
-    <t>ЧЕРНИГОВЪ, съ 1782 году главный городъ Намѣстничества сего имени. Въ ономъ бываетъ въ году четыре ярмарки : первая называемая Проко-фіевская, Іюля съ 8; вторая называемая Евстафіевская, Сентября съ 2о; третія называемая Богоявленская, Генваря съ 7 числа, и продолжаются каждая по недѣлѣ, и четвертый съѣздъ послѣ Свѣтлаго Воскресенія въ десятую пятницу. Торгуютъ на оныхъ многими разными товарами пріѣзжіе изъ Великороссійскихъ и Малороссійскихъ городовъ купцы большею частію Рос-сійскими продуктами ; купечество же города отправляетъ тамошнія произрастѣнія и привозимыя на ярмарки рукодѣлья въ разные Россійскіе города въ немаломъ количествѣ, а особливо по рѣкамъ Деснѣ и Днѣпру.</t>
+    <t>ЧЕРНИГОВЪ, съ 1782 году главный городъ Намѣстничества сего имени. Въ ономъ бываетъ въ году четыре ярмарки : первая называемая Проко-фіевская, Іюля съ 8; вторая называемая Евстафіевская, Сентября съ 20; третія называемая Богоявленская, Генваря съ 7 числа, и продолжаются каждая по недѣлѣ, и четвертый съѣздъ послѣ Свѣтлаго Воскресенія въ десятую пятницу. Торгуютъ на оныхъ многими разными товарами пріѣзжіе изъ Великороссійскихъ и Малороссійскихъ городовъ купцы большею частію Рос-сійскими продуктами ; купечество же города отправляетъ тамошнія произрастѣнія и привозимыя на ярмарки рукодѣлья въ разные Россійскіе города въ немаломъ количествѣ, а особливо по рѣкамъ Деснѣ и Днѣпру.</t>
   </si>
   <si>
     <t>ЧЕРИООСТРОЖСКОЙ НИКОЛАЕВСКОЙ, монастырь Ярославскаго Намѣстничества. При ономъ бываетъ ярмарка Декабря 6, Маія 9 , да о десятой пятницѣ при Соборной церкви Казанскія Богородицы , на память Великомученика Георгія Ноября 26 чиселъ, но токмо знатныхъ товаровъ въ продажѣ не бываетъ, и привозятъ по близости изъ другихъ городовъ по малому числу мѣлочные товары , такожь уѣздные обыватели съѣстные припасы.</t>
@@ -6055,7 +6055,7 @@
     <t>АРХАНГЕЛЬСКЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;главный городъ&lt;/span&gt;&lt;span class="font0"&gt; Намѣстничества сего имени. Въ немъ бываетъ каждой годъ ярмарка , которая начинается въ Маіѣ мѣсяцѣ съ приходомъ изъ Россіи барокъ, а изъ за моря кораблей; прямая же, или валовая начинается всегда въ Іюнѣ, а оканчивается въ первыхъ числахъ Октября ; на ней бываетъ торговля между&lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt; иностранными и Россійскими купцами Россійскими и иностранными товарами , продолжающаяся во время мореплаванія, на которую ярмарку иностранные купцы всякіе иностранные товары чрезъ море на корабляхъ изъ чужихъ краевъ къ Архангельскому порту привозятъ; а Россійскіе въ тѣ мѣста отпускаютъ всякіе привозимые чрезъ верховые города водою и сухимъ путемъ Россійскіе, Китайскіе, Персидскіе, Турецкіе и прочіе Азіатскіе и другіе иностранные товары для народнаго употребленія, а не въ отвозъ въ чужіе край, а именно же: привозимыя вина Французскія, Португальскія, Гишпанскія и Нѣмецкія лучшія и ординарныя, ромъ, уксусъ, водка венгерская, еликсиръ , винной, камень , сукна Голландскія , Аглинскія , Гамбурскія, Шлезскія и прочія лучшія и ординарныя, лоскутья и покроми суконныя , стамеды , штофы и прочія тому подобныя шерстяныя матеріи ; штофы и прочія шелковыя и полушелковыя парчи и ленты , выбойки , полотна Голландскія, олово въ блюдахъ и торѣлкахъ и прочихъ мѣдочахъ , прутовое и въ слиткахъ , свинецъ, желѣзо листовое , иглы , ножи , вилки , ножницы и прочіе желѣзные товары; квасцы, ртуть, сѣра горючая , шелакъ, шпіатеръ, масло деревянное, винныя ягоды , изюмъ , коринка , смоквы, черносливъ, ядры мигдальныя , кофе , чай , перецъ , орѣшки чернильныя , сандалъ, сахаръ, лимоны, померанцы и прочіе фрукты свѣжіе и въ винѣ; гвоздика, корица и прочія пряныя зелья ; канфара, ладонъ росной и простой, изъ гумми разныхъ сортовъ; посуда стеклянная, цѣнинная и каменая , стеклы окончинныя и бутылки , сыры , патока черная, пшено сорочинское , свѣтильня бумажная, бобры, выдры, лисицы; краски , консель брусковая, киноварь, оринакъ; чулки шелковые и шерстяные , также и прочіе отпускные , какъ - то: хлѣбъ , сѣмя льняное, сало говяжье и ворванная смола, юфть, желѣзо полосное и гвозди желѣзные , пенька, ленѣ , рогожи&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span class="font0"&gt;и кульки рогожные ; щетина , канаты и веревки пеньковыя и пакальныя , пряжа канатная, воскъ, гривы конскія , кости , кожи моржевыя , мыло ; мягкая рухлядь , куницы , горнаcтаи , россомахи , бѣлки , песцы, зайчины , мѣхи бѣльи и заячьи &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;, &lt;/span&gt;&lt;span class="font0"&gt;кожи медвежьи, кошечьи и волчьи; полотна гладкія и салфеточныя широкія и узкія и брань уѣздной работы, Фламскія парусныя и равендукъ холстъ , хрящъ, посуда деревянная, свѣчи сальныя, языки говяжьи копченые, губа лиственная , клей Сибирской, кожи подошевныя и ворванныя, сукна сермяжныя и чирковыя туфли, чаи жуланъ и простой, бадьянъ, масло коровье льняное и конопляное, медъ сырецъ, рога оленьи , мясо говяжье соленое , семга соленая , пряники медовые.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>АРХАНГЕЛЬСКОЕ, ЗМѢЕВКА тожь, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Рязанскаго Намѣстничества въ Донковскомъ уѣздѣ ; въ ономъ бываютъ въ году двѣ ярмарки: первая Февраля 2 въ день Срѣтенія Господня , внорая Ноября 8, въ день Архистратига Михаила. Сюда пріѣзжаютъ купцы съ разными мѣлочными. товарами.&lt;/span&gt;</t>
+    <t>АРХАНГЕЛЬСКОЕ, ЗМѢЕВКА тожь, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Рязанскаго Намѣстничества въ Донковскомъ уѣздѣ ; въ ономъ бываютъ въ году двѣ ярмарки: первая Февраля 2 въ день Срѣтенія Господня , вторая Ноября 8, въ день Архистратига Михаила. Сюда пріѣзжаютъ купцы съ разными мѣлочными. товарами.&lt;/span&gt;</t>
   </si>
   <si>
     <t>АСАКОВО , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Тульскаго Намѣстничества въ Веневскомъ уѣздѣ &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;;&lt;/span&gt;&lt;span class="font0"&gt; здѣсь бываетъ годовая ярмарка Іюля 8 числа; пріѣзжаютъ на оную разныхъ городовъ купцы съ товарами.&lt;/span&gt;</t>
@@ -6076,7 +6076,7 @@
     <t>БАЕВКА, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; въ Сибири на вершинѣ рѣки &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;Свіаги&lt;/span&gt;&lt;span class="font0"&gt;; въ ономъ всякое Воскресенье бываетъ торгъ.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>БАЛАКЛЕЕВЪ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко &lt;/span&gt;&lt;span class="font0"&gt;Харьковскаго Намѣстничества въ Изюмовскомъ уѣздѣ. Въ ономъ бываетъ въ году пять ярмарокъ: первая въ недѣлю Ваій, вторая Іюля 12&lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;,&lt;/span&gt;&lt;span class="font0"&gt; третія Августа 1, четвертая Сентября 23, пятая Декабря б чиселъ, на которыя пріѣзжаютъ купцы изъ разныхъ городовъ съ шелковыми , бумажными, гарусными и прочими товарами.&lt;/span&gt;</t>
+    <t>БАЛАКЛЕЕВЪ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко &lt;/span&gt;&lt;span class="font0"&gt;Харьковскаго Намѣстничества въ Изюмовскомъ уѣздѣ. Въ ономъ бываетъ въ году пять ярмарокъ: первая въ недѣлю Ваій, вторая Іюля 12&lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;,&lt;/span&gt;&lt;span class="font0"&gt; третія Августа 1, четвертая Сентября 23, пятая Декабря 6 чиселъ, на которыя пріѣзжаютъ купцы изъ разныхъ городовъ съ шелковыми , бумажными, гарусными и прочими товарами.&lt;/span&gt;</t>
   </si>
   <si>
     <t>БАЛАХНА , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Нижегородскаго Намѣстничества. Въ ономъ бываютъ каждую недѣлю по середамъ и пятницамъ, а въ зимнее время и по воскресеньямъ торги, на которые крестьяне привозятъ болѣе хлѣбъ, съѣстные припасы и разныя для жителей потребности.&lt;/span&gt;</t>
@@ -6085,7 +6085,7 @@
     <t>БАРЫШЕВКА, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко &lt;/span&gt;&lt;span class="font0"&gt;Кіевскаго Намѣстничества въ Переяславскомъ уѣздѣ. Въ ономъ бываютъ въ году три ярмарки: первая Генваря 1, вторая Маія 9, третія Сентября 11 чиселъ, на которыхъ купцы торгуютъ разными мѣлочными товарами и привозимою изъ Донскихъ станицъ мѣлкою рыбою; а жители продаютъ рогатой скотъ, лошадей, хлѣбъ, смолу , горячее вино и Крымскую соль.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>БАСАНЬ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; того же Намѣстничества и уѣзду. Въ ономъ, кромѣ еженедѣльныхъ по понедѣльникамъ торговъ, бываетъ въ году пят&lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;ярмарокъ: первая въ день Вознесенія Господня , вторая въ день Св. Апостоловъ Петра и Павла , третія въ день успенія Пресвятыя Богородицы, четвертая Сентября 2о, въ день Св. Евстафія, пятая Декабря 6, въ день Николая Чудотворца. Торгуютъ на оныхъ разными мѣлочными товарами и привозимою изъ Донскихъ станицъ мѣлкою рыбою. Жители продаютъ рогатой скотъ , лошадей , хлѣбъ, смолу, горячее вино и прочее; также привозятъ сюда для продажи жителямъ Крымскую соль.&lt;/span&gt;&lt;/p&gt;</t>
+    <t>БАСАНЬ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; того же Намѣстничества и уѣзду. Въ ономъ, кромѣ еженедѣльныхъ по понедѣльникамъ торговъ, бываетъ въ году пят&lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;ярмарокъ: первая въ день Вознесенія Господня , вторая въ день Св. Апостоловъ Петра и Павла , третія въ день успенія Пресвятыя Богородицы, четвертая Сентября 20, въ день Св. Евстафія, пятая Декабря 6, въ день Николая Чудотворца. Торгуютъ на оныхъ разными мѣлочными товарами и привозимою изъ Донскихъ станицъ мѣлкою рыбою. Жители продаютъ рогатой скотъ , лошадей , хлѣбъ, смолу, горячее вино и прочее; также привозятъ сюда для продажи жителямъ Крымскую соль.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>БАТРАКЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Синбирскаго Намѣстничества ниже города Сызрани. Въ немъ съ 29 Іюня по 12 Іюля бываетъ годовая ярмарка, на которую особливо привозятъ много уральской рыбы и икры.&lt;/span&gt;</t>
@@ -6145,7 +6145,7 @@
     <t>БОГАЧКА, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; Кіевскаго Намѣстничества въ Миргородскомъ уѣздѣ. Въ ономъ бываетъ въ году двѣ ярмарки : одна въ день Сошествія Святаго Духа, а другая Сентября 1; торгуютъ на оныхъ пріѣзжіе изъ уѣзду жители разными мѣлочными товарами , тамъ родящимися и дѣлающимися, какъ-то хлѣбомъ, горячимъ виномъ,&lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;разнымъ скотомъ, дегтемъ, овчинами, кожами и проч. Иногда пріѣзжаютъ и Великороссійскіе купцы съ краснымъ товаромъ.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>БОГОДУХОВЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Харьковскаго Намѣстничества. Въ ономъ бываетъ въ году шесть ярмарокъ: первая на Сырной недѣлѣ , вторая въ постъ на похвальной недѣлѣ, третія на Вознесеніе , четвертая Іюля 20, пятая Августа 29, шестая Ноября Купцы пріѣзжаютъ на оныя изъ разныхъ Россійскихъ городовъ; привозятъ шелковые товары , парчи , позументы золотые и серебро въ дѣлѣ ; торгуютъ также скотомъ, лошадьми и прочимъ.&lt;/span&gt;</t>
+    <t>БОГОДУХОВЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Харьковскаго Намѣстничества. Въ ономъ бываетъ въ году шесть ярмарокъ: первая на Сырной недѣлѣ , вторая въ постъ на похвальной недѣлѣ, третія на Вознесеніе , четвертая Іюля 20, пятая Августа 29, шестая Ноября 8. Купцы пріѣзжаютъ на оныя изъ разныхъ Россійскихъ городовъ; привозятъ шелковые товары , парчи , позументы золотые и серебро въ дѣлѣ ; торгуютъ также скотомъ, лошадьми и прочимъ.&lt;/span&gt;</t>
   </si>
   <si>
     <t>БОГОРОДИЦКЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ &lt;/span&gt;&lt;span class="font0"&gt;Тульскаго Намѣстничества. Въ семъ городѣ бываетъ ярмарка Іюля 7 и 8 дня, на которую изъ городовъ Тулы , Епифани, Кропивны , Дѣдилова, Ефремова и Донкова привозятъ мѣлочные красные товары , а оныхъ городовъ изъ уѣздовъ крестьяне колесы и лыки.&lt;/span&gt;</t>
@@ -6238,7 +6238,7 @@
     <t>БѢЛАЯ КОЛПЬ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Московской Губерніи въ Волоколамскомъ уѣздѣ. Въ семъ селѣ бываетъ одна въ году ярмарка Августа 19 дня; торгуютъ одинъ день разными крестьянскими товарами.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>БѢЛГОРОДЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Курскаго Намѣстничества. Въ ономъ бываютъ три годовыя ярмарки: первая послѣ Святой недѣли въ десятую пятницу, вторая въ день Апостоловъ Петра и Павла, третія въ день Успвія Богородицы; да въ уѣздѣ онаго города бываютъ годовые торги въ Помѣщичьихъ слободахъ въ Петровской Мацвева, въ Троицкой Матюшкина, въ Сабыниной Брылкиной, въ Шебекиной &lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;Графа Генрикова, въ Алексѣевкѣ , Корчіюкъ тожь, економической &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;,&lt;/span&gt;&lt;span class="font0"&gt; въ Зимовѣйкѣ и Бѣлей Князя Трубецкаго, въ Ефремовкѣ Герсевановой, въ Козмодемьянской Камышина, въ Михайловкѣ , Бекорюковка тожь , Бекорюкова, въ Вознесенской , Ивановка тожь &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;,&lt;/span&gt;&lt;span class="font0"&gt; Бакшеева. Купцы на оные торги пріѣзжаютъ изъ близъ лежащихъ городовъ съ мѣлочными лавочными товарами.&lt;/span&gt;&lt;/p&gt;</t>
+    <t>БѢЛГОРОДЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Курскаго Намѣстничества. Въ ономъ бываютъ три годовыя ярмарки: первая послѣ Святой недѣли въ десятую пятницу, вторая въ день Апостоловъ Петра и Павла, третія въ день Успенія Богородицы; да въ уѣздѣ онаго города бываютъ годовые торги въ Помѣщичьихъ слободахъ въ Петровской Мацвева, въ Троицкой Матюшкина, въ Сабыниной Брылкиной, въ Шебекиной &lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;Графа Генрикова, въ Алексѣевкѣ , Корчіюкъ тожь, економической &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;,&lt;/span&gt;&lt;span class="font0"&gt; въ Зимовѣйкѣ и Бѣлей Князя Трубецкаго, въ Ефремовкѣ Герсевановой, въ Козмодемьянской Камышина, въ Михайловкѣ , Бекорюковка тожь , Бекорюкова, въ Вознесенской , Ивановка тожь &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;,&lt;/span&gt;&lt;span class="font0"&gt; Бакшеева. Купцы на оные торги пріѣзжаютъ изъ близъ лежащихъ городовъ съ мѣлочными лавочными товарами.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>БѢЛИКИ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; Екатеринославскаго Намѣстничества въ Полтавскомъ уѣздѣ. Въ ономъ бываетъ въ году три ярмарки.&lt;/span&gt;</t>
@@ -6376,7 +6376,7 @@
     <t>ВЫБОРЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;пригородъ&lt;/span&gt;&lt;span class="font0"&gt; того же Намѣстничества. Здѣсь бываютъ годовыя ярмарки: первая въ день Сошествія Святаго Духа , вторая въ день Успенія Богородицы, третія въ день Воздвиженія. На оныя пріѣзжаютъ Торопецкіе купцы съ мѣлочнымъ товаромъ.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ВЫБОРГЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;главный городъ &lt;/span&gt;&lt;span class="font0"&gt;Намѣстничества сего имени. Въ ономъ бываетъ въ каждое лѣто ярмарка, какъ въ городѣ приморскомъ; отсюда за море отпускаютъ доски, смолу , желѣзо , а получаютъ соль, табакъ , вина и прочее. Сверхъ сего бываетъ въ году еще двѣ ярмарки: первая Августа 24 вторая Сентября 21, на которыя&lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;крестьяне привозятъ по большей части рогатой скотъ, лошадей и съѣстные припасы.&lt;/span&gt;&lt;/p&gt;</t>
+    <t>ВЫБОРГЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;главный городъ &lt;/span&gt;&lt;span class="font0"&gt;Намѣстничества сего имени. Въ ономъ бываетъ въ каждое лѣто ярмарка, какъ въ городѣ приморскомъ; отсюда за море отпускаютъ доски, смолу , желѣзо , а получаютъ соль, табакъ , вина и прочее. Сверхъ сего бываетъ въ году еще двѣ ярмарки: первая Августа 24, вторая Сентября 21, на которыя&lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;крестьяне привозятъ по большей части рогатой скотъ, лошадей и съѣстные припасы.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>ВЫСОКОЕ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Московской Губерніи въ Волоколамскомъ уѣздѣ , въ которомъ есть небольшой рядъ , и въ ономъ производится продажа всякаго щепетильнаго товару, деревянной посуды , хлѣба и хмѣлю,&lt;/span&gt;</t>
@@ -6391,7 +6391,7 @@
     <t>ВЫЧУГА, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Костромскаго Намѣстничества въ уѣздѣ города Кинешмы. Здѣсь бываетъ годовая ярмарка въ Троицынъ день.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ВЫШГОРОДЪ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;пригородъ&lt;/span&gt;&lt;span class="font0"&gt; Псковскаго Намѣстничества. Въ ономъ бываетъ въ году двѣ ярмарки : первая въ день, Бориса и Глѣба, а другая въ день Рождества Іоанна Предтечи.&lt;/span&gt;</t>
+    <t>ВЫШГОРОДЪ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;пригородъ&lt;/span&gt;&lt;span class="font0"&gt; Псковскаго Намѣстничества. Въ ономъ бываетъ въ году двѣ ярмарки : первая въ день Бориса и Глѣба, а другая въ день Рождества Іоанна Предтечи.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ВЫШГОРОДЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Московской Губерніи въ Верейскомъ уѣздѣ. Въ ономъ бываютъ двѣ ярмарки въ году: первая въ десятую пятницу , вторая Іюля 2 числа ; на оныя пріѣзжаютъ купцы изъ городовъ Вереи, Можайска и Боровска , и множество сходится крестьянства ; торгуютъ всякими съѣстными припасами и крестьянскимъ товаромъ, какъ-то колесами, дегтемъ и тому подобнымъ.&lt;/span&gt;</t>
@@ -6442,7 +6442,7 @@
     <t>ГЖАТЬ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Смоленскаго Намѣстничества. Въ семъ городѣ бываетъ годовая ярмарка , сверхъ каждонедѣльныхъ торговъ, Іюля 8 дня ; а въ селахъ бываетъ съѣздъ въ храмовые праздники , и въ каждомъ на одинъ только тотъ день.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ГЛЕМЯЗОВЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; Кіевскаго Намѣстничества въ Переяславскомъ уѣздѣ. Въ ономъ бываетъ въ году четыре ярмарки : первая на Сырной недѣлѣ, вторая въ день Прополовенія, третія въ день Преображенія, четвертая въ день Введенія. Купцы пріѣзжаютъ на оныя изъ близъ лежащихъ городовъ съ красными крамными и прочими товарами, съ стеклянною и деревянною посудою, съ мѣлкою изъ Донскихъ станицѣ рыбою; жители продаютъ рогатой скотъ , лошадей, хлѣбѣ, смолу, горячее вино и прочее; привозятъ также сюда для продажи жителямъ Крымскую соль.&lt;/span&gt;</t>
+    <t>ГЛЕМЯЗОВЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; Кіевскаго Намѣстничества въ Переяславскомъ уѣздѣ. Въ ономъ бываетъ въ году четыре ярмарки : первая на Сырной недѣлѣ, вторая въ день Преполовенія, третія въ день Преображенія, четвертая въ день Введенія. Купцы пріѣзжаютъ на оныя изъ близъ лежащихъ городовъ съ красными крамными и прочими товарами, съ стеклянною и деревянною посудою, съ мѣлкою изъ Донскихъ станицѣ рыбою; жители продаютъ рогатой скотъ , лошадей, хлѣбѣ, смолу, горячее вино и прочее; привозятъ также сюда для продажи жителямъ Крымскую соль.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ГЛИНСКЪ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;слобода&lt;/span&gt;&lt;span class="font0"&gt; Екатеринославскаго Намѣстничества. Въ оной бываетъ въ году три ярмарки.&lt;/span&gt;</t>
@@ -6562,13 +6562,13 @@
     <t>ДМИТРОВЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Московской Губерніи. Въ ономъ бываетъ въ году одна ярмарка, которая начинается съ 15 Сентября , и продолжается недѣлю ; съ товарами пріѣзжаютъ изъ разныхъ ближиихъ городовъ , а именно изъ Москвы ,&lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;изъ Переславля Залѣснаго , изъ Ярославля; изъ Катина и изъ смѣжныхъ мѣстъ. Товары оные состоятъ въ щепетьѣ, шапкахъ, сапогахъ и прочей всякой мѣлочи; также торговыхъ дней въ недѣлѣ бываетъ два: понедѣльникъ и четвер токъ.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>ДМИТРОВКА, ОЛЬШАНКА тожь , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Кіевскаго Намѣстничества около слободы Яб унева. Бываетъ здѣсь одна годовая ярмарка, на которую купцы пріѣзжаютъ съ разными товарами.&lt;/span&gt;</t>
+    <t>ДМИТРОВКА, ОЛЬШАНКА тожь , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Кіевскаго Намѣстничества около слободы Яблунева. Бываетъ здѣсь одна годовая ярмарка, на которую купцы пріѣзжаютъ съ разными товарами.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ДМИТРОВСКАЯ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;крѣпость &lt;/span&gt;&lt;span class="font0"&gt;Екатеринославскаго Намѣстничества. Въ оной бываетъ въ году три ярмарки.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ДОБРАЯ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;слобода&lt;/span&gt;&lt;span class="font0"&gt; Воронежскаго Намѣстничества. Въ сей слободѣ въ году бываютъ три небольшія ярмарки: первая 9 Маія, вторая 26 Іюня, третія б Декабря, и продолжаются не болѣе какъ по одному, или по два Дни. Купцы на оныя привозятъ мѣлочные товары.&lt;/span&gt;</t>
+    <t>ДОБРАЯ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;слобода&lt;/span&gt;&lt;span class="font0"&gt; Воронежскаго Намѣстничества. Въ сей слободѣ въ году бываютъ три небольшія ярмарки: первая 9 Маія, вторая 26 Іюня, третія 6 Декабря, и продолжаются не болѣе какъ по одному, или по два Дни. Купцы на оныя привозятъ мѣлочные товары.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ДОМНИЦКОЙ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;монастырь &lt;/span&gt;&lt;span class="font0"&gt;Черниговскаго Намѣстничества и уѣзду. При ономъ. бываетъ&lt;/span&gt;</t>
@@ -6694,7 +6694,7 @@
     <t>ЗЕМЛЯНСКЪ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Воронежскаго Намѣстничества. Въ уѣздѣ сего города бываютъ ярмарки въ году въ трехъ селахъ; на оныя пріѣзжаютъ разныхъ городовъ Россійскіе купцы съ мѣлкимъ товаромъ.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ЗИНКОВЪ, или ЗѢНКОВЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Черниговскаго Намѣстничества. Въ ономъ бываетъ въ годъ четыре ярмарки : первая Іюня 25 , въ день С. Іоанна Крестителя , вторая 15 Августа , въ день успенія Пресвятыя Богородицы, третія Октября 1, въ день Покрова Пресвятыя Богородицы , четвертая Декабря б, въ день Святителя Николая. На оныхъ торгуютъ разнымъ скотомъ, хлѣбомъ и съѣстными припасами. Здѣсь бываютъ и еженедѣльные торжки въ понедѣльникъ и пятокъ, и торгуютъ на оныхъ хлѣбомъ.&lt;/span&gt;</t>
+    <t>ЗИНКОВЪ, или ЗѢНКОВЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Черниговскаго Намѣстничества. Въ ономъ бываетъ въ годъ четыре ярмарки : первая Іюня 25 , въ день С. Іоанна Крестителя , вторая 15 Августа , въ день успенія Пресвятыя Богородицы, третія Октября 1, въ день Покрова Пресвятыя Богородицы , четвертая Декабря 6, въ день Святителя Николая. На оныхъ торгуютъ разнымъ скотомъ, хлѣбомъ и съѣстными припасами. Здѣсь бываютъ и еженедѣльные торжки въ понедѣльникъ и пятокъ, и торгуютъ на оныхъ хлѣбомъ.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ЗМѢЕВѢ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;слобода&lt;/span&gt;&lt;span class="font0"&gt; Харьковскаго Намѣстничества въ уѣздѣ города Изюма. Въ оной бываютъ въ году три ярмарки : первая Іюня 29, въ день Св. Апостоловъ Петра и Павла, вторая Сентября 1, въ день Симеона Столпника, третія Октября 14, на день Параскевы. Купцы пріѣзжаютъ на оныя изъ разныхъ Россійскихъ городовъ съ шелковыми , шерстяными , бумажными и прочими товарами.&lt;/span&gt;</t>
@@ -6703,10 +6703,10 @@
     <t>ЗМѢТНЕВЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Новогородскаго - Сѣверскаго Намѣстничества въ Сосницкомъ уѣздѣ. Обыватели онаго имѣютъ изрядной промыслъ бобрами , выдрами и рыбною въ Деснѣ ловлею.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ЗОЛОТОНОША , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Кіевскаго Намѣстничества. Въ немъ бываетъ въ году четыре ярмарки: первая въ Ѳомину недѣлю , вторая въ день Сошествія Свитаго Духа, третія въ день Рождества Богородицы , четвертая Декабря 6. Купцы пріѣзжаютъ на оныя изъ близъ лежащихъ городовъ съ красными крамными и прочими товарами , стеклянною и деревянною посудою и мѣлкою изъ Донскихъ станицъ рыбою; жители продаютъ рогатой скотъ, лошадей , хлѣбъ , смолу, горячее &lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;вино и прочее; привозятъ также сюда для лродажи жителямъ Крымскую соль.&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>ЗОЛОЧЕВЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Харьковскаго Намѣстничества. Здѣсь бываютъ ярмарки Іюня 29, Августа 6, Декабря б ; торгуютъ купцы мѣлочнымъ товаромъ, виномъ, пивомъ, медомъ и прочимъ.&lt;/span&gt;</t>
+    <t>ЗОЛОТОНОША , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Кіевскаго Намѣстничества. Въ немъ бываетъ въ году четыре ярмарки: первая въ Ѳомину недѣлю , вторая въ день Сошествія Святаго Духа, третія въ день Рождества Богородицы , четвертая Декабря 6. Купцы пріѣзжаютъ на оныя изъ близъ лежащихъ городовъ съ красными крамными и прочими товарами , стеклянною и деревянною посудою и мѣлкою изъ Донскихъ станицъ рыбою; жители продаютъ рогатой скотъ, лошадей , хлѣбъ , смолу, горячее &lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;вино и прочее; привозятъ также сюда для лродажи жителямъ Крымскую соль.&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>ЗОЛОЧЕВЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Харьковскаго Намѣстничества. Здѣсь бываютъ ярмарки Іюня 29, Августа 6, Декабря 6 ; торгуютъ купцы мѣлочнымъ товаромъ, виномъ, пивомъ, медомъ и прочимъ.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ЗУБЦОВЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Тверскаго Намѣстничества. Въ семъ городѣ бываютъ годовыя ярмарки : первая въ десятую пятницу по Пасхѣ , вторая Іюля 20, въ день Пророка Іліи, третія Августа 6, въ день Преображенія , четвертая Августа 15, въ день успенія , пятая 6 Декабря, шестая Маія 9, въ день Чудотворца Николая, седьмая Генваря 7, въ день Крестителя Іоанна, осьмая на Сырной недѣлѣ въ среду; торгуютъ окрестныхъ городовъ купцы - шелковыми , бумажными и прочими мѣлочными товарами, а большею частію съѣстными припасами.&lt;/span&gt;</t>
@@ -6751,7 +6751,7 @@
     <t>ИЗМАЙЛОВО , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Нижегородскаго Намѣстничества въ Арсамазскомъ уѣздѣ. Въ ономъ бываетъ одна въ г Ду ярмарка.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ИЗЮМЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Харьковскаго Намѣстничества. Въ семъ городѣ бываетъ въ году четыре ярмарки: первая въ Маіѣ мѣсяцѣ въ день Преполовенія, вторая Іюня 24, въ день Рождества Іоанна Предтечи, третія Сентября 14, въ день Воздвиженія честнаго Креста, четвертая Октября 2б, въ день Великомученика Димитрія ; на оныя купцы пріѣзжаютъ изъ разныхъ городовъ съ шелковыми , бумажными , шерстяными и прочими товарами.&lt;/span&gt;</t>
+    <t>ИЗЮМЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Харьковскаго Намѣстничества. Въ семъ городѣ бываетъ въ году четыре ярмарки: первая въ Маіѣ мѣсяцѣ въ день Преполовенія, вторая Іюня 24, въ день Рождества Іоанна Предтечи, третія Сентября 14, въ день Воздвиженія честнаго Креста, четвертая Октября 26, въ день Великомученика Димитрія ; на оныя купцы пріѣзжаютъ изъ разныхъ городовъ съ шелковыми , бумажными , шерстяными и прочими товарами.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ИЛЬИНСКОЕ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Тульскаго Намѣстничества въ Каширскомъ уѣздѣ. Здѣсь бываютъ торжки каждонедѣльно въ пятничные дни ; товары на оные привозятъ изъ уѣзда холсты льняные разные, да изъ городовъ Ярославля, Переславля Залѣснаго и Углича пріѣзжаютъ купцы съ мѣлочными всякими небогатыми товарами.&lt;/span&gt;</t>
@@ -6805,7 +6805,7 @@
     <t>КАМЕНЕЦЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; Полотскаго Намѣстничества въ уѣздѣ города Динабурга. Въ семъ. мѣстѣ бываютъ три ярмарки въ году; торгуютъ Рижскаго &lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;Дворца крестьяне разными мѣлочными товарами, виномъ и пивомъ.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>КАМЕНКА , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;слобода&lt;/span&gt;&lt;span class="font0"&gt; Харьковскаго Намѣстничества въ уѣздѣ города Изюма. Въ оной бываетъ въ году четыре ярмарки: первая ьъ день Алексія человѣка Божія , вторая въ день Великомученика Георгія, третія и четвертая во дни Николая Чудотворца лѣтняго и зимняго. На оныя купцы пріѣзжаютъ изъ разныхъ Россійскихъ городовъ съ шелковыми , бумажными , шерстяными товарами и прочимъ.&lt;/span&gt;</t>
+    <t>КАМЕНКА , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;слобода&lt;/span&gt;&lt;span class="font0"&gt; Харьковскаго Намѣстничества въ уѣздѣ города Изюма. Въ оной бываетъ въ году четыре ярмарки: первая въ день Алексія человѣка Божія , вторая въ день Великомученика Георгія, третія и четвертая во дни Николая Чудотворца лѣтняго и зимняго. На оныя купцы пріѣзжаютъ изъ разныхъ Россійскихъ городовъ съ шелковыми , бумажными , шерстяными товарами и прочимъ.&lt;/span&gt;</t>
   </si>
   <si>
     <t>КАМЫШНЯ, или КОМЫШНЯ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; Кіевскаго Настничества въ Миргородскомъ уѣздѣ. Въ ономъ бываетъ въ году три ярмарки: первая въ недѣлю Ваій , вторая въ десятую послѣ Свѣтлаго Воскресенія пятницу , третія 26 Октября , въ день Св. Димитрія. На оныхъ торгуютъ рогатымъ скотомъ и лошадьми, а на еженедѣльныхъ въ понедѣльникъ и пятницу торгахъ торгуютъ пріѣзжіе изъ окольныхъ мѣстъ хлѣбомъ и съѣстными припасами.&lt;/span&gt;</t>
@@ -7210,7 +7210,7 @@
     <t>МАЛОЙ АРХАНГЕЛЬСКЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Орловскаго Намѣстничества. Въ немъ бываетъ дважды въ недѣлю съѣздъ.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>МАЛОЙ ЯРОСЛАВЕЦЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Калужскаго Намѣстничества. Въ немъ бываютъ въ годъ ярмарки Апрѣля 23, Маія 9, Ноября 26, Декабря б и въ десятую пятницу по Пасхѣ , на которыя пріѣзжаютъ купцы изъ Боровска, Вереи и Серпухова съ шелковыми и бумажными платками , китайками , выбойками, чаемъ, сахаромъ, кофіемъ и разными москотильными товарами ; а главную часть сего торгу составляютъ окрестные жители, которые привозятъ съѣстные припасы и деревенскія издѣлья.&lt;/span&gt;</t>
+    <t>МАЛОЙ ЯРОСЛАВЕЦЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Калужскаго Намѣстничества. Въ немъ бываютъ въ годъ ярмарки Апрѣля 23, Маія 9, Ноября 26, Декабря 6 и въ десятую пятницу по Пасхѣ , на которыя пріѣзжаютъ купцы изъ Боровска, Вереи и Серпухова съ шелковыми и бумажными платками , китайками , выбойками, чаемъ, сахаромъ, кофіемъ и разными москотильными товарами ; а главную часть сего торгу составляютъ окрестные жители, которые привозятъ съѣстные припасы и деревенскія издѣлья.&lt;/span&gt;</t>
   </si>
   <si>
     <t>МАЛЫКОВА, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; Полотскаго Намѣстничества въ уѣздѣ города Динабурга. Въ семъ мѣстѣ бываетъ въ году одна ярмарка; торгуютъ Рижскаго Дворца крестьяне разными мѣлочными товарами, виномъ и пивомъ.&lt;/span&gt;</t>
@@ -7258,7 +7258,7 @@
     <t>МЕРЕХВА, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; Харьковскаго Намѣстничества и уѣзду. Здѣсь бываютъ ярмарки Іюня 24, Августа 6; торгуютъ купцы мѣлочными, товарами , виномъ, пивомъ, медомъ и прочимъ.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>МЕХОНСКОЙ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;острогъ &lt;/span&gt;&lt;span class="font0"&gt;Уфимскаго Намѣстничества въ Челябинскомъ уѣздѣ. Здѣсь бываетъ ярмарка Декабря 25 и Іюля 2о; торгуютъ мѣлочнымъ товаромъ.&lt;/span&gt;</t>
+    <t>МЕХОНСКОЙ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;острогъ &lt;/span&gt;&lt;span class="font0"&gt;Уфимскаго Намѣстничества въ Челябинскомъ уѣздѣ. Здѣсь бываетъ ярмарка Декабря 25 и Іюля 20; торгуютъ мѣлочнымъ товаромъ.&lt;/span&gt;</t>
   </si>
   <si>
     <t>МЕЩОВСКЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Калужскаго Намѣстничества, Здѣсь бываетъ одна въ году ярмарка Іюля 29 дня; торгъ продолжается три дни ; на оную пріѣзжаютъ изъ разныхъ городовъ купцы со всякими товарами, а по большей части крестьяне съ Пенькою и хлѣбомъ.&lt;/span&gt;</t>
@@ -7378,7 +7378,7 @@
     <t>НАСПИЩИ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Тульскаго Намѣстничества въ уѣздѣ города Алексина. Здѣсь бываетъ ярмарка Маія 2 и Іюля 24 дня; торгуютъ купцы до крестьянъ надлежащими товарами.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>НЕВЕЛЬ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Полотскаго Намѣстничества. Въ немъ бываютъ въ году четыре ярмарки: первая въ день Богоявленія, вторая въ первую недѣлю великаго поста, третія въ пятокъ Пктъ днемъ Пророка Иліи, четвертая Декабря 6 дня.&lt;/span&gt;</t>
+    <t>НЕВЕЛЬ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Полотскаго Намѣстничества. Въ немъ бываютъ въ году четыре ярмарки: первая въ день Богоявленія, вторая въ первую недѣлю великаго поста, третія въ пятокъ предъ днемъ Пророка Иліи, четвертая Декабря 6 дня.&lt;/span&gt;</t>
   </si>
   <si>
     <t>НЕЛЬЯНСКОЙ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;желѣзной заводъ&lt;/span&gt;&lt;span class="font0"&gt; Пермскаго Намѣстничества въ Екатеринбургскомъ уѣздѣ. Здѣсь бываетъ въ день Святыхъ Апостоловъ Петра и Павла нарочитая ярмарка прoдолжающаяся нѣсколько дней на которую съѣзжается много купцовъ изъ близъ лежащихъ городовъ , а именно: Екатеринбурга , Верхотурья, Туринска, Тюмени , которые , какъ и тамошніе жители , разными Россійскими , Сибирскими и Китайскими товарами торгуютъ.&lt;/span&gt;</t>
@@ -7471,7 +7471,7 @@
     <t>ОПОЧКА, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Псковскаго Намѣстничества. Въ семъ городѣ бываетъ въ году три ярмарки.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ОПОШНОЕ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; Черниговскаго Намѣстничества въ Гадяцкомъ уѣздѣ. Въ ономъ бываетъ въ году четыре ярмарки : первая въ недѣлю Ѳомину, вторая въ десятую пятницу, третія Августа б, въ день Преображенія Господня, четвертая Октября 29, въ день Св. Димитрія ; на оныхъ торгуютъ разнымъ скотомъ, хлѣбомъ и съѣстными припасами. Здѣсь бываютъ еженедѣльные торжки въ понедѣльникъ и пятокъ, и торгуютъ большею частію хлѣбомъ.&lt;/span&gt;</t>
+    <t>ОПОШНОЕ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; Черниговскаго Намѣстничества въ Гадяцкомъ уѣздѣ. Въ ономъ бываетъ въ году четыре ярмарки : первая въ недѣлю Ѳомину, вторая въ десятую пятницу, третія Августа 6, въ день Преображенія Господня, четвертая Октября 29, въ день Св. Димитрія ; на оныхъ торгуютъ разнымъ скотомъ, хлѣбомъ и съѣстными припасами. Здѣсь бываютъ еженедѣльные торжки въ понедѣльникъ и пятокъ, и торгуютъ большею частію хлѣбомъ.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ОПУШКА, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;отчина&lt;/span&gt;&lt;span class="font0"&gt; разныхъ Господъ Тамбовскаго Намѣстничества въ Шатскомъ уѣздѣ. Здѣсь бываетъ въ году ярмарка 8 Іюля; торгуютъ разными товарами , какъ - то пенькою , разнымъ холстомъ медомъ, саломъ и прочимъ.&lt;/span&gt;</t>
@@ -7540,7 +7540,7 @@
     <t>ПЕРЕВОЛОЧНА, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; Екатеринославскаго Намѣстничества. Въ ономъ бываетъ въ году двѣ ярмарки.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ПЕРЕКОПЕЦЪ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; въ уѣздѣ города Харькова. Здѣсь бываетъ ярмарка Марта 9, Маія б и Ноября 8, торгуютъ купцы мѣлочными товарами, виномъ , пивомъ , медомъ и прочимъ.&lt;/span&gt;</t>
+    <t>ПЕРЕКОПЕЦЪ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; въ уѣздѣ города Харькова. Здѣсь бываетъ ярмарка Марта 9, Маія 6 и Ноября 8, торгуютъ купцы мѣлочными товарами, виномъ , пивомъ , медомъ и прочимъ.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ПЕРЕМЫШЛЬ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Калужскаго Намѣстничества. Здѣсь бываетъ годовая ярмарка сверхъ обыкновенныхъ торговъ въ десятую пятницу по Пасхѣ; привозятъ на продажу хдѣбъ, пеньку , хмѣль и прочее.&lt;/span&gt;</t>
@@ -7576,7 +7576,7 @@
     <t>ПЕТРОВСКОЕ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Орловскаго Намѣстничества въ Елецкомъ уѣздѣ. Здѣсь бываетъ ярмарка Іюня 19 числа; на оной торгуютъ Елецкіе купцы и другихъ городовъ съ уѣздными обывателями всякими разными мѣлочными товарами; а обыватели продаютъ купцамъ и своей братьи лошадей, скотину, холстъ и съѣстные всякіе припасы и рукодѣлье.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ПЕТРОМА, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Ярославскаго Намѣстничества въ Пошехонскомъ уѣздѣ. Въ ономъ бываютъ двѣ годовыя ярмарки: первая Троецкая, вторая Ивановская , то есть 26 Сентября; пріѣзжаютъ на оныя купцы изъ сосѣдственныхъ городовъ съ разными шелковыми мѣлочными и прочими товарами.&lt;/span&gt;</t>
+    <t>ПЕТРОМА, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Ярославскаго Намѣстничества въ Пошехонскомъ уѣздѣ. Въ ономъ бываютъ двѣ годовыя ярмарки: первая Троицкая, вторая Ивановская , то есть 26 Сентября; пріѣзжаютъ на оныя купцы изъ сосѣдственныхъ городовъ съ разными шелковыми мѣлочными и прочими товарами.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ПЕТРОПАВЛОВСКОЙ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;шанцъ&lt;/span&gt;&lt;span class="font0"&gt; Екатеринославскаго Намѣстничества. Въ ономъ бываетъ въ годъ четыре ярмарки.&lt;/span&gt;</t>
@@ -7636,7 +7636,7 @@
     <t>ПОЛТАВА , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Екатеринославскаго Намѣстничества. Въ ономъ бываетъ въ году четыре ярмарки : первая въ сплошную недѣлю , вторая Маія 9, Николаевская , третія Іюля 20, Ильинская, четвертая Сентября 14, Воздвиженская. На оныя пріѣзжаютъ Великороссійскіе , Малороссійскіе и иностранные , изъ Польши , Шлезіи, Гданска, Царя - Града и изъ всей Турецкой области купцы и промышленники со всякими знатными и мѣлочными товарами. Купечество сего города отправляетъ во всѣ оныя мѣста родящіеся у нихъ и въ уѣздѣ продукты, какъ - то скотъ &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;,&lt;/span&gt;&lt;span class="font0"&gt; масло , лошадей и другіе , холстъ, канаты и пушные разнаго рода товары. На еженедѣльные торги собираются въ оной городъ уѣздные жители, и торгуютъ Россійскими продуктами.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ПОНОРНИЦА , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко &lt;/span&gt;&lt;span class="font0"&gt;Черниговскаго Намѣстничества и уѣзду. Въ ономъ бываетъ въ году Двѣ ярмарки : первая Апрѣля 23, вторая Сентября чиселъ; торгуютъ на оныхъ и еженедѣльныхъ торгахъ пріѣзжіе изъ ближнихъ городовъ купцы мѣлочными товарами , а&lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt; &lt;/span&gt;&lt;span class="font0"&gt;окольные жители тутошними произрастаніями и рукодѣліемъ, какъ - то деревянною посудою, неводными нитками , также скотомъ и прочими съѣстными припасами.&lt;/span&gt;</t>
+    <t>ПОНОРНИЦА , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко &lt;/span&gt;&lt;span class="font0"&gt;Черниговскаго Намѣстничества и уѣзду. Въ ономъ бываетъ въ году Двѣ ярмарки : первая Апрѣля 23, вторая Сентября 8 чиселъ; торгуютъ на оныхъ и еженедѣльныхъ торгахъ пріѣзжіе изъ ближнихъ городовъ купцы мѣлочными товарами , а&lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt; &lt;/span&gt;&lt;span class="font0"&gt;окольные жители тутошними произрастаніями и рукодѣліемъ, какъ - то деревянною посудою, неводными нитками , также скотомъ и прочими съѣстными припасами.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ПОРѢЧЬЕ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Смоленскаго Намѣстничества. Въ ономъ бываетъ въ году двѣ ярмарки : первая Іюня мѣсяца въ десятую пятницу, вторая Сентября 8, въ день Рождества Богородицы ; купцы пріѣзжаютъ изъ близъ лежащихъ городовъ съ разными товарами.&lt;/span&gt;</t>
@@ -7648,7 +7648,7 @@
     <t>ПОТОКЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; Кіевскаго Намѣстничества въ Миргородскомъ уѣздѣ. Въ ономъ&lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;бываютъ въ годъ двѣ ярмарки: дпа Іюня 24, а другая Октября 6 чиселъ. Торгуютъ на оныхъ пріѣзжіе изъ уѣзду жители разными мѣлочными товарами , дамъ родящимися и дѣлающимися, какъ - то хлѣбомъ, горячимъ виномъ, разнымъ скотомъ, овчинами, кожами и проч. Иногда пріѣзжаютъ и Великороссійскіе купцы съ краснымъ товаромъ.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>ПОЧИНКИ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Пензенскаго Намѣстничества въ Саранскомъ уѣздѣ. Бываетъ здѣсь ярмарка въ послѣднихъ числахъ юля; привозятъ купцы разные мѣлочные шелковые товары.&lt;/span&gt;</t>
+    <t>ПОЧИНКИ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Пензенскаго Намѣстничества въ Саранскомъ уѣздѣ. Бываетъ здѣсь ярмарка въ послѣднихъ числахъ Іюля; привозятъ купцы разные мѣлочные шелковые товары.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ПОЧИНКИ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Нижегородскаго Намѣстничества. Въ емъ, кромѣ еженедѣльнаго по четвергамъ торгу, бываетъ въ одъ Маія 25 дня ярмарка, на вторую пріѣзжаютъ изъ ближнихъ городовъ купцы съ мѣлочными шелковыми товарами, крестьяне привозить бывшею  хлѣбъ, лѣсъ и деревянную посуду.&lt;/span&gt;</t>
@@ -7702,7 +7702,7 @@
     <t>РАМЕНЬЕ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Московской Губерніи въ Волоколамскомъ уѣздѣ. Здѣсь бываютъ въ году ярмарки Іюня 24 и 18 Сентября ; торгуютъ по одному дню разными крестьянскими товарами.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>РАТКОВКА, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;слобода&lt;/span&gt;&lt;span class="font0"&gt; Харьковскаго Намѣстничества въ уѣздѣ города Изюма. Въ оной бываютъ въ году три ярмарки: Первая на Вознесеніе Господне , вторая Августа б , на Преображеніе , третія Октября 1, въ день Покрова. Купцы на оныя пріѣзжаютъ изъ разныхъ городовъ съ шелковыми , бумажными , гарусными и прочими товарами.&lt;/span&gt;</t>
+    <t>РАТКОВКА, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;слобода&lt;/span&gt;&lt;span class="font0"&gt; Харьковскаго Намѣстничества въ уѣздѣ города Изюма. Въ оной бываютъ въ году три ярмарки: Первая на Вознесеніе Господне , вторая Августа 6 , на Преображеніе , третія Октября 1, въ день Покрова. Купцы на оныя пріѣзжаютъ изъ разныхъ городовъ съ шелковыми , бумажными , гарусными и прочими товарами.&lt;/span&gt;</t>
   </si>
   <si>
     <t>РАТСБУРГЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;отчина&lt;/span&gt;&lt;span class="font0"&gt; Меньшикова въ Екатеринославскомъ Намѣстничествѣ. Здѣсь бываютъ двѣ ярмарки , а именно : первая Троицкая, которая прежде &lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;была въ Лебединскомъ Троицкомъ монастырѣ , и переведена въ тое отчину; а другая въ той же отчинѣ Покровская , Октября і дня ; да сверхъ того бываютъ понедѣльные и временные торжки , на кои пріѣзжаютъ изъ ближнихъ городовъ купцы и изъ уѣздовъ крестьяне съ хлѣбомъ и прочею мѣлочью.&lt;/span&gt;&lt;/p&gt;</t>
@@ -8020,7 +8020,7 @@
     <t>ТЕПЛОГОРСКАЯ БОГОРОДИЦКАЯ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;пустыня&lt;/span&gt;&lt;span class="font0"&gt; Вологодскаго Намѣстничества въ уѣздѣ Устюга Великаго. Здѣсь бываетъ въ году одна ярмарка, на которую пріѣзжаютъ купцы изъ разныхъ городовъ по большей части съ мѣлочными товарами.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ТЕРЕШКОВО, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Тверскаго Намѣстничества въ Зубцовскомъ уѣздѣ. Въ немъ бываетъ годовая ярмарка Маія 2о, въ день Алексѣя Митрополита; на оную пріѣзжаютъ купцы изъ окрестныхъ ближнихъ городовъ съ мѣлочными шелковыми и прочими товарами.&lt;/span&gt;</t>
+    <t>ТЕРЕШКОВО, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Тверскаго Намѣстничества въ Зубцовскомъ уѣздѣ. Въ немъ бываетъ годовая ярмарка Маія 20, въ день Алексѣя Митрополита; на оную пріѣзжаютъ купцы изъ окрестныхъ ближнихъ городовъ съ мѣлочными шелковыми и прочими товарами.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ТЕРЯЕВО, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Московской Губерніи въ Рузскомъ уѣздѣ. Въ немъ бываетъ годовая ярмарка въ день Святаго Пророка Иліи.&lt;/span&gt;</t>
@@ -8053,7 +8053,7 @@
     <t>ТОМАРОВКА, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;слобода&lt;/span&gt;&lt;span class="font0"&gt; въ уѣздѣ города Карпова. Въ оной бываетъ ярмарка послѣ Рождества на всеѣдной недѣлѣ въ пятницу, Маія 9, Іюля 8, Декабря 6, и продолжаются оныя по одному дню. Купцы пріѣзжаютъ изъ окрестныхъ городовъ съ мѣлочными товарами.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ТОРЖОКЪ, съ 1775 году &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Тверскаго Намѣстничества. Здѣсь бываютъ въ году три ярмарки : первая Генваря 6, вторая первой недѣли великаго&lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;ста въ Воскресенье, третія Сентября 15 числа.   &lt;/span&gt;&lt;/p&gt;</t>
+    <t>ТОРЖОКЪ, съ 1775 году &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Тверскаго Намѣстничества. Здѣсь бываютъ въ году три ярмарки : первая Генваря 6, вторая первой недѣли великаго&lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;поста въ Воскресенье, третія Сентября 15 числа.   &lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>ТОРОПЕЦЪ, съ 1777 году &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Псковскаго Намѣстничества. Въ немъ случается въ году одна указная ярмарка въ Iюлѣ мѣсяцѣ въ пятокъ, предъ праздникомъ Пророка Иліи, на которую по большей части съѣзжаются крестьяне изъ ближнихъ деревень съ мѣлочнымъ крестьянскимъ товаромъ и рукодельемъ.&lt;/span&gt;</t>
@@ -8086,7 +8086,7 @@
     <t>ТУЛА, съ 1777 году главный &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Намѣстничества сего имени. Здѣсь ярмарка бываетъ въ году два раза: I) при церкви Покрова Пресвятыя Богородицы , въ десятую отъ Святой недѣли пятницу; вторая Іюня 8 дня, при состоящемъ за городовымъ замкомъ Казанскомъ Соборѣ. Для складки привозимыхъ товаровъ имѣются подъ Тульскимъ Магистратомъ въ нижнемъ департаментѣ, также и особь построенныя палатки. Съ товарами на ярмарки постороннаго съѣзда не бываетъ, а отправляются только тамошними. Въ недѣлѣ два торга, въ понедѣльникъ и четвертокъ.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ТУРЕЦКАЯ &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;треть,&lt;/span&gt;&lt;span class="font0"&gt; или &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;волость&lt;/span&gt;&lt;span class="font0"&gt; Вологодскаго Намѣстничества въ уѣздѣ города Яренска. Здѣсь бываетъ ярмарка Февраля съ 15 дня по Мартъ мѣсяцъ; скупаютъ здѣсь купцы по большей части заготовленную и свезенную сюда крестьянами рыбу.&lt;/span&gt;</t>
+    <t>ТУРЕЦКАЯ &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;треть,&lt;/span&gt;&lt;span class="font0"&gt; или &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;волость&lt;/span&gt;&lt;span class="font0"&gt; Вологодскаго Намѣстничества въ уѣздѣ города Яренска. Здѣсь бываетъ ярмарка Февраля съ 15 дня по Мартѣ мѣсяцъ; скупаютъ здѣсь купцы по большей части заготовленную и свезенную сюда крестьянами рыбу.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ТУРИНСКЪ, съ 1782 году &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Тобольскаго Намѣстничества. Здѣсь бываютъ знатные торговые съѣзды по вся воскресные дни.&lt;/span&gt;</t>
@@ -8209,7 +8209,7 @@
     <t>ХРУЩОВО, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Рязанскаго Намѣстничества въ уѣздѣ города Донкова. Здѣсь бываютъ въ году двѣ ярмарки: первая Маія 9, вторая Августа 16 дня; пріѣзжаютъ на оныя купцы съ разными мѣлочными товарами , также и крестьянство.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ЦАРЕВЪ БОРИСОВЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городокъ&lt;/span&gt;&lt;span class="font0"&gt; Харьковскаго Намѣстничества въ уѣздѣ города Изюма. Въ ономъ бываетъ въ году четыре ярмарки : первая на всеѣдной недѣлѣ, вторая въ недѣлю Мѵроносицъ , третія послѣ Святой недѣли въ девятую пятницу, четвертая Ноября 8, въ день Архистратига Михаила; купцы пріѣзжаютъ на оныя изъ разныхъ Россійскихъ городовъ съ шелковыми , бумажными , гарусными и прочими товарами.&lt;/span&gt;</t>
+    <t>ЦАРЕВЪ БОРИСОВЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городокъ&lt;/span&gt;&lt;span class="font0"&gt; Харьковскаго Намѣстничества въ уѣздѣ города Изюма. Въ ономъ бываетъ въ году четыре ярмарки : первая на всеѣдной недѣлѣ, вторая въ недѣлю Мироносицъ , третія послѣ Святой недѣли въ девятую пятницу, четвертая Ноября 8, въ день Архистратига Михаила; купцы пріѣзжаютъ на оныя изъ разныхъ Россійскихъ городовъ съ шелковыми , бумажными , гарусными и прочими товарами.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ЦАРИЧЕНКА , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко &lt;/span&gt;&lt;span class="font0"&gt;Екатеринославскаго Намѣстничества въ Полтавскомъ уѣздѣ. Въ ономъ бываютъ въ году три ярмарки.&lt;/span&gt;</t>
@@ -8236,7 +8236,7 @@
     <t>ЧАУСЫ, съ 1778 году &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Могилевскаго Намѣстничества Здѣсь бываетъ одна годовая ярмарка.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ЧЕЛЯБИНСКЪ, съ 1782 году &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Уфимскаго Намѣстничества , лежащій на рѣкѣ &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;Міясѣ,&lt;/span&gt;&lt;span class="font0"&gt; отъ Далматовскаго монастыря во стѣ пятидесяти четырехъ верстахъ, въ самой срединѣ Башкирцевъ, можетъ со временемъ вразсужденіи торговъ сдѣлаться знатнымъ мѣстомъ; ибо намѣреніе принято было нетокмо для большей способности ради Башкирцевъ тамъ завести ярмарку, но еще и купечество изъ Великой Бухаріи, какъ въ Оренбургъ, такъ отчасти и туда перевести. Здѣсь бываютъ въ году двѣ ярмарки: первая Маія 9, вторая Декабря б дня.&lt;/span&gt;</t>
+    <t>ЧЕЛЯБИНСКЪ, съ 1782 году &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Уфимскаго Намѣстничества , лежащій на рѣкѣ &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;Міясѣ,&lt;/span&gt;&lt;span class="font0"&gt; отъ Далматовскаго монастыря во стѣ пятидесяти четырехъ верстахъ, въ самой срединѣ Башкирцевъ, можетъ со временемъ вразсужденіи торговъ сдѣлаться знатнымъ мѣстомъ; ибо намѣреніе принято было нетокмо для большей способности ради Башкирцевъ тамъ завести ярмарку, но еще и купечество изъ Великой Бухаріи, какъ въ Оренбургъ, такъ отчасти и туда перевести. Здѣсь бываютъ въ году двѣ ярмарки: первая Маія 9, вторая Декабря 6 дня.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ЧЕНБАРЪ, съ 1780 году &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Пензенскаго Намѣстничества. Въ ономъ бываетъ въ году ярмарка въ десятую пятницу &lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;по Пасхѣ; купцы пріѣзжаютъ изъ близъ лежащихъ городовъ съ недорогими товарами.&lt;/span&gt;&lt;/p&gt;</t>
@@ -8260,7 +8260,7 @@
     <t>ЧЕРНАВСКЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;слобода&lt;/span&gt;&lt;span class="font0"&gt; Воронежскаго Намѣстничества. Здѣсь бываетъ одна въ году ярмарка въ день Срѣтенія Иконы Владимірскія Богородицы , то есть Іюня 23 дня; на оную пріѣзжаютъ купцы изъ ближнихъ городовъ съ мѣлкими товарами, и продолжается оная только половину дня.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ЧЕРНИГОВЪ, съ 1782 году &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;главный городъ&lt;/span&gt;&lt;span class="font0"&gt; Намѣстничества сего имени. Въ ономъ бываетъ въ году четыре ярмарки : первая называемая Проко-фіевская, Іюля съ 8; вторая называемая Евстафіевская, Сентября съ 2о; третія называемая Богоявленская, Генваря съ 7 числа, и продолжаются каждая по недѣлѣ, и четвертый съѣздъ послѣ Свѣтлаго Воскресенія въ десятую пятницу. Торгуютъ на оныхъ многими разными товарами пріѣзжіе изъ Великороссійскихъ и Малороссійскихъ городовъ купцы большею частію Рос-&lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;сійскими продуктами ; купечество же города отправляетъ тамошнія произрастѣнія и привозимыя на ярмарки рукодѣлья въ разные Россійскіе города въ немаломъ количествѣ, а особливо по рѣкамъ Деснѣ и Днѣпру.&lt;/span&gt;&lt;/p&gt;</t>
+    <t>ЧЕРНИГОВЪ, съ 1782 году &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;главный городъ&lt;/span&gt;&lt;span class="font0"&gt; Намѣстничества сего имени. Въ ономъ бываетъ въ году четыре ярмарки : первая называемая Проко-фіевская, Іюля съ 8; вторая называемая Евстафіевская, Сентября съ 20; третія называемая Богоявленская, Генваря съ 7 числа, и продолжаются каждая по недѣлѣ, и четвертый съѣздъ послѣ Свѣтлаго Воскресенія въ десятую пятницу. Торгуютъ на оныхъ многими разными товарами пріѣзжіе изъ Великороссійскихъ и Малороссійскихъ городовъ купцы большею частію Рос-&lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;сійскими продуктами ; купечество же города отправляетъ тамошнія произрастѣнія и привозимыя на ярмарки рукодѣлья въ разные Россійскіе города въ немаломъ количествѣ, а особливо по рѣкамъ Деснѣ и Днѣпру.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>ЧЕРИООСТРОЖСКОЙ НИКОЛАЕВСКОЙ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;монастырь&lt;/span&gt;&lt;span class="font0"&gt; Ярославскаго Намѣстничества. При ономъ бываетъ ярмарка Декабря 6, Маія 9 , да о десятой пятницѣ при Соборной церкви Казанскія Богородицы , на память Великомученика Георгія Ноября 26 чиселъ, но токмо знатныхъ товаровъ въ продажѣ не бываетъ, и привозятъ по близости изъ другихъ городовъ по малому числу мѣлочные товары , такожь уѣздные обыватели съѣстные припасы.&lt;/span&gt;</t>

</xml_diff>

<commit_message>
reran text processing on updated text
</commit_message>
<xml_diff>
--- a/output/process/no_geo.xlsx
+++ b/output/process/no_geo.xlsx
@@ -3589,7 +3589,7 @@
     <t>ВЕЛИЖЪ, городъ Полотскаго Намѣстничества. Въ семъ городѣ бываетъ въ году двѣ ярмарки : первая 20 Іюля , вторая на первой недѣлѣ великаго поста.</t>
   </si>
   <si>
-    <t>ВЕЛИКОЕ, село Ярославскаго Намѣстничества въ Ростовскомъ уѣздѣ. Въ ономъ бываетъ</t>
+    <t>ВЕЛИКОЕ, село Ярославскаго Намѣстничества въ Ростовскомъ уѣздѣ. Въ ономъ бываетъ годовая ярмарка Сентября 8 числа ; пріѣзжаютъ купцы изъ Ярославля , Юрьева и изъ Переславля Залѣскаго съ суровскими товарами.</t>
   </si>
   <si>
     <t>ВЕНДЕНЪ, городъ Рижскаго Намѣстничества. Здѣсь бываютъ въ году двѣ ярмарки: одна въ Ивановъ , а другая въ Михайловъ день; но оныя въ себѣ важнаго ничего не заключаютъ.</t>
@@ -3868,7 +3868,7 @@
     <t>ДОБРАЯ, слобода Воронежскаго Намѣстничества. Въ сей слободѣ въ году бываютъ три небольшія ярмарки: первая 9 Маія, вторая 26 Іюня, третія 6 Декабря, и продолжаются не болѣе какъ по одному, или по два Дни. Купцы на оныя привозятъ мѣлочные товары.</t>
   </si>
   <si>
-    <t>ДОМНИЦКОЙ, монастырь Черниговскаго Намѣстничества и уѣзду. При ономъ. бываетъ</t>
+    <t>ДОМНИЦКОЙ, монастырь Черниговскаго Намѣстничества и уѣзду. При ономъ. бываетъ двѣ въ году ярмарки: первая послѣ Пасхи въ десятую пятницу , а другая Сентября 8 дня.</t>
   </si>
   <si>
     <t>ДОНКОВЪ, городъ Рязанскаго Намѣстничества. Бываютъ здѣсь двѣ въ году ярмарки : первая въ пятницу десятой , вторая въ пятницу второй надесять недѣли по Пасхѣ. Пріѣзжаютъ на оныя купцы съ разными мѣлочными товарами.</t>
@@ -4036,7 +4036,7 @@
     <t>ИВАНОВЦЫ, шанцъ Екатеринославскаго Намѣстничества. Въ ономъ бываютъ въ году двѣ ярмарки.</t>
   </si>
   <si>
-    <t>ИВИЦА , слобода Курскаго Намѣстничества въ Короченскомъ уѣздѣ. Въ оной бываетъ въ году двѣ ярмарки: первая</t>
+    <t>ИВИЦА , слобода Курскаго Намѣстничества въ Короченскомъ уѣздѣ. Въ оной бываетъ въ году двѣ ярмарки: первая Іюня 29, вторая Іюля 20 дня; на оныя купцы пріѣзжаютъ съ разными товарами.</t>
   </si>
   <si>
     <t>ИГРИЩИ , село Ярославскаго Намѣстничества и уѣзду. Въ семъ селѣ бываетъ годовая ярмарка въ Сентябрѣ мѣсяцѣ ; съѣзжаются купцы изъ ближнихъ городовъ, какъ - то Ярославля, Ростова , Романова , Углича , Борисоглѣбска , Рыбнаго , Мологи и слободы Норской.</t>
@@ -4486,7 +4486,7 @@
     <t>ЛЯДЫ, мѣстечко Могилевскаго Намѣстничества въ Оршанскомъ уѣздѣ. Здѣсь бываетъ въ году двѣ ярмарки.</t>
   </si>
   <si>
-    <t>ЛЯУДЕРА , мѣстечко Полотскаго Намѣстничества въ уѣздѣ города Динабурга. Въ семъ мѣстѣ бываютъ въ году двѣ ярмарки ; торгуютъ Рижскаго Дверца крестьяне разными мѣлочными товарами, виномъ и ливомъ.</t>
+    <t>ЛЯУДЕРА , мѣстечко Полотскаго Намѣстничества въ уѣздѣ города Динабурга. Въ семъ мѣстѣ бываютъ въ году двѣ ярмарки ; торгуютъ Рижскаго Дверца крестьяне разными мѣлочными товарами, виномъ и пивомъ.</t>
   </si>
   <si>
     <t>МАКАЛОВО, село Пензенскаго Намѣстничества въ уѣздѣ города Краснослободска. Здѣсь бываетъ одна въ году ярмарка на десятой недѣлѣ по Пасхѣ въ пятокъ; но сюда пріѣзжаютъ по большей части крестьяне съ своими припасами.</t>
@@ -4519,7 +4519,7 @@
     <t>МАРКУШЕВСКАЯ , Економическая деревня Архангельскаго Намѣстничества. Здѣсь бываетъ ярмарка Іюля 8 дня; купцы пріѣзжаютъ изъ ближнихъ городовъ съ разными мѣлочными москотильными и прочими товарами, и покупаютъ у крестъянъ ихъ пріуготовленія, а иногда и мягкую рухлядь, также сало , холстъ и прочее.</t>
   </si>
   <si>
-    <t>МАСЛЕНСКАЯ, слобода Уфимскаго Намѣстничества въ Челябинскомъ уѣздѣ. Здѣсь бы</t>
+    <t>МАСЛЕНСКАЯ, слобода Уфимскаго Намѣстничества въ Челябинскомъ уѣздѣ. Здѣсь бываетъ ярмарка Декабря 25 и Іюля 20 дня ; торгуютъ на оныхъ мѣлочнымъ товаромъ.</t>
   </si>
   <si>
     <t>МАСЛОВИЧИ, мѣстечко Могилевскаго Намѣстничества въ Мстиславскомъ уѣздѣ. Здѣсь бываетъ одна ярмарка въ году.</t>
@@ -4567,7 +4567,7 @@
     <t>МИЛОСЛАВИЧИ, мѣстечко Могилевскаго Намѣстничества въ Климовицкомъ уѣздѣ. Въ ономъ бываетъ одна годовая ярмарка.</t>
   </si>
   <si>
-    <t>МИРГОРОДЪ , городъ Кіевскаго Намѣстничества. Въ ономъ бываетъ въ году четыре ярмарки: первая на срединѣ великаго поста , другая въ день праздника Вознесенія Христова , третія Сентября 8 , четвертая Декабря 6 чиселъ; торгуютъ ва оныхъ пріѣзжіе изъ уѣзду жители разными мѣдкими товарами , тамъ родящимися и дѣлающимися, какъ - то хлѣбомъ , горячимъ виномъ, разнымъ скотомъ, овчинами , кожами ; иногда пріѣзжаютъ и Великороссійскіе купцы съ краснымъ товаромъ и прочимъ.</t>
+    <t>МИРГОРОДЪ , городъ Кіевскаго Намѣстничества. Въ ономъ бываетъ въ году четыре ярмарки: первая на срединѣ великаго поста , другая въ день праздника Вознесенія Христова , третія Сентября 8 , четвертая Декабря 6 чиселъ; торгуютъ ва оныхъ пріѣзжіе изъ уѣзду жители разными мѣлкими товарами , тамъ родящимися и дѣлающимися, какъ - то хлѣбомъ , горячимъ виномъ, разнымъ скотомъ, овчинами , кожами ; иногда пріѣзжаютъ и Великороссійскіе купцы съ краснымъ товаромъ и прочимъ.</t>
   </si>
   <si>
     <t>МИРОПОЛЬЕ, городъ Харьковскаго Намѣстничества. Въ семъ городѣ бываютъ въ году три ярмарки : первая на пятой недѣлѣ великаго поста, вторая на седьмой недѣлѣ по Пасхѣ, третія Сентября 1 дня. На оныя пріѣзжаютъ купцы изъ ближнихъ Великороссійскихъ городовъ , и привозятъ всякіе внутренніе мѣлкіе товары, торгуютъ также скотомъ и лошадьми.</t>
@@ -5686,7 +5686,7 @@
     <t>ЯРАНСКЪ, съ 1781 году городъ Вятскаго Намѣстничества. Въ немъ бываютъ каждонедѣльно по Воскресеньямъ съѣзды , на которыхъ купцы торгуютъ разными шелковыми и бумажными мѣлочными, также привозимыми изъ уѣзду, воскомъ, медомъ, саломъ, кожами, овчинами , хмѣлемъ и разными здѣшняго произрастѣнія пушными товарами.</t>
   </si>
   <si>
-    <t>ЯРЕНСКЪ, съ 1780 году городъ Вологодскаго Намѣстничества. Въ ономъ бываетъ въ году одинъ небольшой торгъ Генваря отъ 18 по 23 день раз-ными мѣлочными товарами, на которой пріѣзжаютъ купцы изъ Устюга Великаго, Вологды и Соли-Вычегодской.</t>
+    <t>ЯРЕНСКЪ, съ 1780 году городъ Вологодскаго Намѣстничества. Въ ономъ бываетъ въ году одинъ небольшой торгъ Генваря отъ 18 по 23 день разными мѣлочными товарами, на которой пріѣзжаютъ купцы изъ Устюга Великаго, Вологды и Соли-Вычегодской.</t>
   </si>
   <si>
     <t>ЯРЕСКИ, мѣстечко Кіевскаго Намѣстничества въ Миргородскомъ уѣздѣ. Въ ономъ бываетъ въ году двѣ ярмарки: первая Іюня 24, другая Августа 15; торгуютъ на оныхъ пріѣзжіе изъ уѣздовъ жители разными мѣлочными товарами , тамъ родящимися, какъ-то хлѣбомъ , горячимъ виномъ, разнымъ скотомъ, овчинами, кожами и прочимъ; иногда пріѣзжаютъ и Великороссійскіе купцы съ краснымъ товаромъ.</t>
@@ -6304,7 +6304,7 @@
     <t>БѢЛАЯ КОЛПЬ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Московской Губерніи въ Волоколамскомъ уѣздѣ. Въ семъ селѣ бываетъ одна въ году ярмарка Августа 19 дня; торгуютъ одинъ день разными крестьянскими товарами.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>БѢЛГОРОДЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Курскаго Намѣстничества. Въ ономъ бываютъ три годовыя ярмарки: первая послѣ Святой недѣли въ десятую пятницу, вторая въ день Апостоловъ Петра и Павла, третія въ день Успенія Богородицы; да въ уѣздѣ онаго города бываютъ годовые торги въ Помѣщичьихъ слободахъ въ Петровской Мацвева, въ Троицкой Матюшкина, въ Сабыниной Брылкиной, въ Шебекиной &lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;Графа Генрикова, въ Алексѣевкѣ , Корчіюкъ тожь, економической &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;,&lt;/span&gt;&lt;span class="font0"&gt; въ Зимовѣйкѣ и Бѣлей Князя Трубецкаго, въ Ефремовкѣ Герсевановой, въ Козмодемьянской Камышина, въ Михайловкѣ , Бекорюковка тожь , Бекорюкова, въ Вознесенской , Ивановка тожь &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;,&lt;/span&gt;&lt;span class="font0"&gt; Бакшеева. Купцы на оные торги пріѣзжаютъ изъ близъ лежащихъ городовъ съ мѣлочными лавочными товарами.&lt;/span&gt;&lt;/p&gt;</t>
+    <t>БѢЛГОРОДЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Курскаго Намѣстничества. Въ ономъ бываютъ три годовыя ярмарки: первая послѣ Святой недѣли въ десятую пятницу, вторая въ день Апостоловъ Петра и Павла, третія въ день Успенія Богородицы; да въ уѣздѣ онаго города бываютъ годовые торги въ Помѣщичьихъ слободахъ въ Петровской Мацвева, въ Троицкой Матюшкина, въ Сабыниной Брылкиной, въ Шебекиной &lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;Графа Генрикова, въ Алексѣевкѣ , Корчіюкъ тожь, економической , въ Зимовѣйкѣ и Бѣлей Князя Трубецкаго, въ Ефремовкѣ Герсевановой, въ Козмодемьянской Камышина, въ Михайловкѣ , Бекорюковка тожь , Бекорюкова, въ Вознесенской , Ивановка тожь , Бакшеева. Купцы на оные торги пріѣзжаютъ изъ близъ лежащихъ городовъ съ мѣлочными лавочными товарами.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>БѢЛИКИ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; Екатеринославскаго Намѣстничества въ Полтавскомъ уѣздѣ. Въ ономъ бываетъ въ году три ярмарки.&lt;/span&gt;</t>
@@ -6358,7 +6358,7 @@
     <t>ВЕЛИЖЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Полотскаго Намѣстничества. Въ семъ городѣ бываетъ въ году двѣ ярмарки : первая 20 Іюля , вторая на первой недѣлѣ великаго поста.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ВЕЛИКОЕ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Ярославскаго Намѣстничества въ Ростовскомъ уѣздѣ. Въ ономъ бываетъ&lt;/span&gt;</t>
+    <t>ВЕЛИКОЕ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Ярославскаго Намѣстничества въ Ростовскомъ уѣздѣ. Въ ономъ бываетъ годовая ярмарка Сентября 8 числа ; пріѣзжаютъ купцы изъ Ярославля , Юрьева и изъ Переславля Залѣскаго съ суровскими товарами.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ВЕНДЕНЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Рижскаго Намѣстничества. Здѣсь бываютъ въ году двѣ ярмарки: одна въ Ивановъ , а другая въ Михайловъ день; но оныя въ себѣ важнаго ничего не заключаютъ.&lt;/span&gt;</t>
@@ -6637,7 +6637,7 @@
     <t>ДОБРАЯ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;слобода&lt;/span&gt;&lt;span class="font0"&gt; Воронежскаго Намѣстничества. Въ сей слободѣ въ году бываютъ три небольшія ярмарки: первая 9 Маія, вторая 26 Іюня, третія 6 Декабря, и продолжаются не болѣе какъ по одному, или по два Дни. Купцы на оныя привозятъ мѣлочные товары.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ДОМНИЦКОЙ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;монастырь &lt;/span&gt;&lt;span class="font0"&gt;Черниговскаго Намѣстничества и уѣзду. При ономъ. бываетъ&lt;/span&gt;</t>
+    <t>ДОМНИЦКОЙ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;монастырь &lt;/span&gt;&lt;span class="font0"&gt;Черниговскаго Намѣстничества и уѣзду. При ономъ. бываетъ двѣ въ году ярмарки: первая послѣ Пасхи въ десятую пятницу , а другая Сентября 8 дня.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ДОНКОВЪ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Рязанскаго Намѣстничества. Бываютъ здѣсь двѣ въ году ярмарки : первая въ пятницу десятой , вторая въ пятницу второй надесять недѣли по Пасхѣ. Пріѣзжаютъ на оныя купцы съ разными мѣлочными товарами.&lt;/span&gt;</t>
@@ -6805,7 +6805,7 @@
     <t>ИВАНОВЦЫ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;шанцъ&lt;/span&gt;&lt;span class="font0"&gt; Екатеринославскаго Намѣстничества. Въ ономъ бываютъ въ году двѣ ярмарки.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ИВИЦА , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;слобода&lt;/span&gt;&lt;span class="font0"&gt; Курскаго Намѣстничества въ Короченскомъ уѣздѣ. Въ оной бываетъ въ году двѣ ярмарки: первая&lt;/span&gt;</t>
+    <t>ИВИЦА , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;слобода&lt;/span&gt;&lt;span class="font0"&gt; Курскаго Намѣстничества въ Короченскомъ уѣздѣ. Въ оной бываетъ въ году двѣ ярмарки: первая Іюня 29, вторая Іюля 20 дня; на оныя купцы пріѣзжаютъ съ разными товарами.&lt;/span&gt;</t>
   </si>
   <si>
     <t>ИГРИЩИ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Ярославскаго Намѣстничества и уѣзду. Въ семъ селѣ бываетъ годовая ярмарка въ Сентябрѣ мѣсяцѣ ; съѣзжаются купцы изъ ближнихъ &lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;городовъ, какъ - то Ярославля, Ростова , Романова , Углича , Борисоглѣбска , Рыбнаго , Мологи и слободы Норской.&lt;/span&gt;&lt;/p&gt;</t>
@@ -7255,7 +7255,7 @@
     <t>ЛЯДЫ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; Могилевскаго Намѣстничества въ Оршанскомъ уѣздѣ. Здѣсь бываетъ въ году двѣ ярмарки.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ЛЯУДЕРА , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; Полотскаго Намѣстничества въ уѣздѣ города Динабурга. Въ семъ мѣстѣ бываютъ въ году двѣ ярмарки ; торгуютъ Рижскаго Дверца крестьяне разными мѣлочными товарами, виномъ и ливомъ.&lt;/span&gt;</t>
+    <t>ЛЯУДЕРА , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; Полотскаго Намѣстничества въ уѣздѣ города Динабурга. Въ семъ мѣстѣ бываютъ въ году двѣ ярмарки ; торгуютъ Рижскаго Дверца крестьяне разными мѣлочными товарами, виномъ и пивомъ.&lt;/span&gt;</t>
   </si>
   <si>
     <t>МАКАЛОВО, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;село&lt;/span&gt;&lt;span class="font0"&gt; Пензенскаго Намѣстничества въ уѣздѣ города Краснослободска. Здѣсь бываетъ одна въ году ярмарка на десятой недѣлѣ по Пасхѣ въ пятокъ; но сюда пріѣзжаютъ по большей части крестьяне съ своими припасами.&lt;/span&gt;</t>
@@ -7288,7 +7288,7 @@
     <t>МАРКУШЕВСКАЯ , Економическая &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;деревня&lt;/span&gt;&lt;span class="font0"&gt; Архангельскаго Намѣстничества. Здѣсь бываетъ ярмарка Іюля 8 дня; купцы пріѣзжаютъ изъ ближнихъ городовъ съ разными мѣлочными москотильными и прочими товарами, и покупаютъ у крестъ&lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;янъ ихъ пріуготовленія, а иногда и мягкую рухлядь, также сало , холстъ и прочее.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>МАСЛЕНСКАЯ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;слобода &lt;/span&gt;&lt;span class="font0"&gt;Уфимскаго Намѣстничества въ Челябинскомъ уѣздѣ. Здѣсь бы&lt;/span&gt;</t>
+    <t>МАСЛЕНСКАЯ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;слобода &lt;/span&gt;&lt;span class="font0"&gt;Уфимскаго Намѣстничества въ Челябинскомъ уѣздѣ. Здѣсь бываетъ ярмарка Декабря 25 и Іюля 20 дня ; торгуютъ на оныхъ мѣлочнымъ товаромъ.&lt;/span&gt;</t>
   </si>
   <si>
     <t>МАСЛОВИЧИ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко &lt;/span&gt;&lt;span class="font0"&gt;Могилевскаго Намѣстничества въ Мстиславскомъ уѣздѣ. Здѣсь бываетъ одна ярмарка въ году.&lt;/span&gt;</t>
@@ -7336,7 +7336,7 @@
     <t>МИЛОСЛАВИЧИ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко &lt;/span&gt;&lt;span class="font0"&gt;Могилевскаго Намѣстничества въ Климовицкомъ уѣздѣ. Въ ономъ бываетъ одна годовая ярмарка.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>МИРГОРОДЪ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Кіевскаго Намѣстничества. Въ ономъ бываетъ въ году четыре ярмарки: первая на срединѣ великаго поста , другая въ день праздника Вознесенія Христова , третія Сентября 8 , четвертая Декабря 6 чиселъ; торгуютъ ва оныхъ пріѣзжіе изъ уѣзду жители разными мѣдкими товарами , тамъ родящимися и дѣлающимися, какъ - то хлѣбомъ , горячимъ виномъ, разнымъ скотомъ, овчинами , кожами ; иногда пріѣзжаютъ и Великороссійскіе купцы съ краснымъ товаромъ и прочимъ.&lt;/span&gt;</t>
+    <t>МИРГОРОДЪ , &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Кіевскаго Намѣстничества. Въ ономъ бываетъ въ году четыре ярмарки: первая на срединѣ великаго поста , другая въ день праздника Вознесенія Христова , третія Сентября 8 , четвертая Декабря 6 чиселъ; торгуютъ ва оныхъ пріѣзжіе изъ уѣзду жители разными мѣлкими товарами , тамъ родящимися и дѣлающимися, какъ - то хлѣбомъ , горячимъ виномъ, разнымъ скотомъ, овчинами , кожами ; иногда пріѣзжаютъ и Великороссійскіе купцы съ краснымъ товаромъ и прочимъ.&lt;/span&gt;</t>
   </si>
   <si>
     <t>МИРОПОЛЬЕ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Харьковскаго Намѣстничества. Въ семъ городѣ бываютъ въ году три ярмарки : первая на пятой недѣлѣ великаго поста, вторая на седьмой недѣлѣ по Пасхѣ, третія Сентября 1 дня. На оныя пріѣзжаютъ купцы изъ ближнихъ Великороссійскихъ городовъ , и привозятъ всякіе внутренніе мѣлкіе товары, торгуютъ также скотомъ и лошадьми.&lt;/span&gt;</t>
@@ -8455,7 +8455,7 @@
     <t>ЯРАНСКЪ, съ 1781 году &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Вятскаго Намѣстничества. Въ немъ бываютъ каждонедѣльно по Воскресеньямъ съѣзды , на которыхъ купцы торгуютъ разными шелковыми и бумажными мѣлочными, также привозимыми изъ уѣзду, воскомъ, медомъ, саломъ, кожами, овчинами , хмѣлемъ и разными здѣшняго произрастѣнія пушными товарами.&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ЯРЕНСКЪ, съ 1780 году &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Вологодскаго Намѣстничества. &lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;Въ ономъ бываетъ въ году одинъ небольшой торгъ Генваря отъ 18 по 23 день раз-ными мѣлочными товарами, на которой пріѣзжаютъ купцы изъ Устюга Великаго, Вологды и Соли-Вычегодской.&lt;/span&gt;&lt;/p&gt;</t>
+    <t>ЯРЕНСКЪ, съ 1780 году &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;городъ&lt;/span&gt;&lt;span class="font0"&gt; Вологодскаго Намѣстничества. &lt;/span&gt;&lt;p&gt;&lt;span class="font0"&gt;Въ ономъ бываетъ въ году одинъ небольшой торгъ Генваря отъ 18 по 23 день разными мѣлочными товарами, на которой пріѣзжаютъ купцы изъ Устюга Великаго, Вологды и Соли-Вычегодской.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>ЯРЕСКИ, &lt;/span&gt;&lt;span class="font0" style="font-style:italic;"&gt;мѣстечко&lt;/span&gt;&lt;span class="font0"&gt; Кіевскаго Намѣстничества въ Миргородскомъ уѣздѣ. Въ ономъ бываетъ въ году двѣ ярмарки: первая Іюня 24, другая Августа 15; торгуютъ на оныхъ пріѣзжіе изъ уѣздовъ жители разными мѣлочными товарами , тамъ родящимися, какъ-то хлѣбомъ , горячимъ виномъ, разнымъ скотомъ, овчинами, кожами и прочимъ; иногда пріѣзжаютъ и Великороссійскіе купцы съ краснымъ товаромъ.&lt;/span&gt;</t>

</xml_diff>